<commit_message>
Adding missing ids for localization in principles
</commit_message>
<xml_diff>
--- a/UX-Guide-Metadata/draft/localizations/crosscheck strings epub-onix-canonical_json.xlsx
+++ b/UX-Guide-Metadata/draft/localizations/crosscheck strings epub-onix-canonical_json.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/greg/Git/publ-a11y/UX-Guide-Metadata/draft/localizations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F21357E3-10C6-6C4D-AF9D-564D33F74315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7762EC5C-8E96-774B-8CAB-52C2551F99BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17160" xr2:uid="{2FB70C81-061D-D945-B60D-ABB2568C93DD}"/>
   </bookViews>
@@ -18,6 +18,9 @@
     <sheet name="epub-metadata-strings" sheetId="5" r:id="rId3"/>
     <sheet name="onix-metadata-strings" sheetId="8" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">crosscheck!$A$1:$D$90</definedName>
+  </definedNames>
   <calcPr calcId="191029" iterate="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -61,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="244">
   <si>
     <t>id</t>
   </si>
@@ -775,6 +778,24 @@
   </si>
   <si>
     <t>hasards-explanatory</t>
+  </si>
+  <si>
+    <t>This publication exceeds accepted accessibility standards.</t>
+  </si>
+  <si>
+    <t>The publication contains a conformance statement that it meets the EPUB Accessibility and WCAG 2 Level AAA standard.</t>
+  </si>
+  <si>
+    <t>The publication contains a conformance statement that it meets the EPUB Accessibility and WCAG 2 Level AA standard.</t>
+  </si>
+  <si>
+    <t>The publication contains a conformance statement that it meets the EPUB Accessibility and WCAG 2 Level A standard.</t>
+  </si>
+  <si>
+    <t>The publication does not include a conformance statement.</t>
+  </si>
+  <si>
+    <t>The conformance metadata is missing and conformity to a standard of this publication is unknown.</t>
   </si>
 </sst>
 </file>
@@ -830,27 +851,7 @@
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1231,11 +1232,11 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2:A90">_xlfn.UNIQUE(_xlfn.VSTACK('principles-string'!D2:D84,'epub-metadata-strings'!D2:D71,'onix-metadata-strings'!D2:D67))</f>
+        <f t="array" ref="A2:A90">_xlfn.UNIQUE(_xlfn.VSTACK('principles-string'!D2:D94,'epub-metadata-strings'!D2:D71,'onix-metadata-strings'!D2:D67))</f>
         <v>visual-adjustments-title</v>
       </c>
       <c r="B2" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A2),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A2&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A2&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A2)</f>
         <v>1</v>
       </c>
       <c r="C2" s="3">
@@ -1252,7 +1253,7 @@
         <v>visual-adjustments-modifiable</v>
       </c>
       <c r="B3" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A3),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A3&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A3&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A3)</f>
         <v>2</v>
       </c>
       <c r="C3" s="3">
@@ -1269,7 +1270,7 @@
         <v>visual-adjustments-unmodifiable</v>
       </c>
       <c r="B4" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A4),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A4&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A4&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A4)</f>
         <v>2</v>
       </c>
       <c r="C4" s="3">
@@ -1286,7 +1287,7 @@
         <v>visual-adjustments-unknown</v>
       </c>
       <c r="B5" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A5),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A5&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A5&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A5)</f>
         <v>2</v>
       </c>
       <c r="C5" s="3">
@@ -1303,7 +1304,7 @@
         <v>nonvisual-reading-title</v>
       </c>
       <c r="B6" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A6),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A6&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A6&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A6)</f>
         <v>1</v>
       </c>
       <c r="C6" s="3">
@@ -1320,7 +1321,7 @@
         <v>nonvisual-reading-readable</v>
       </c>
       <c r="B7" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A7),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A7&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A7&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A7)</f>
         <v>2</v>
       </c>
       <c r="C7" s="3">
@@ -1337,7 +1338,7 @@
         <v>nonvisual-reading-may-not-fully</v>
       </c>
       <c r="B8" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A8),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A8&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A8&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A8)</f>
         <v>2</v>
       </c>
       <c r="C8" s="3">
@@ -1354,7 +1355,7 @@
         <v>nonvisual-reading-not-fully</v>
       </c>
       <c r="B9" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A9),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A9&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A9&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A9)</f>
         <v>2</v>
       </c>
       <c r="C9" s="3">
@@ -1371,7 +1372,7 @@
         <v>nonvisual-reading-unknown</v>
       </c>
       <c r="B10" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A10),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A10&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A10&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A10)</f>
         <v>2</v>
       </c>
       <c r="C10" s="3">
@@ -1388,7 +1389,7 @@
         <v>conformance-title</v>
       </c>
       <c r="B11" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A11),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A11&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A11&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A11)</f>
         <v>1</v>
       </c>
       <c r="C11" s="3">
@@ -1402,11 +1403,11 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="str">
-        <v>conformance-aa</v>
+        <v>conformance-aaa</v>
       </c>
       <c r="B12" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A12),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A12&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A12&amp;"-compact"))</f>
-        <v>1</v>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A12)</f>
+        <v>2</v>
       </c>
       <c r="C12" s="3">
         <f>COUNTIF('epub-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A12,"-compact", ""),"-descriptive", ""))</f>
@@ -1419,11 +1420,11 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" t="str">
-        <v>conformance-certification-info</v>
+        <v>conformance-aa</v>
       </c>
       <c r="B13" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A13),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A13&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A13&amp;"-compact"))</f>
-        <v>4</v>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A13)</f>
+        <v>3</v>
       </c>
       <c r="C13" s="3">
         <f>COUNTIF('epub-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A13,"-compact", ""),"-descriptive", ""))</f>
@@ -1436,11 +1437,11 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="str">
-        <v>conformance-certifier-prefix</v>
+        <v>conformance-a</v>
       </c>
       <c r="B14" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A14),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A14&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A14&amp;"-compact"))</f>
-        <v>4</v>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A14)</f>
+        <v>3</v>
       </c>
       <c r="C14" s="3">
         <f>COUNTIF('epub-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A14,"-compact", ""),"-descriptive", ""))</f>
@@ -1453,11 +1454,11 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="str">
-        <v>conformance-certifier-credentials-prefix</v>
+        <v>conformance-no</v>
       </c>
       <c r="B15" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A15),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A15&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A15&amp;"-compact"))</f>
-        <v>3</v>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A15)</f>
+        <v>2</v>
       </c>
       <c r="C15" s="3">
         <f>COUNTIF('epub-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A15,"-compact", ""),"-descriptive", ""))</f>
@@ -1470,11 +1471,11 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" t="str">
-        <v>conformance-details</v>
+        <v>conformance-certification-info</v>
       </c>
       <c r="B16" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A16),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A16&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A16&amp;"-compact"))</f>
-        <v>2</v>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A16)</f>
+        <v>4</v>
       </c>
       <c r="C16" s="3">
         <f>COUNTIF('epub-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A16,"-compact", ""),"-descriptive", ""))</f>
@@ -1487,11 +1488,11 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="str">
-        <v>conformance-claim</v>
+        <v>conformance-certifier-prefix</v>
       </c>
       <c r="B17" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A17),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A17&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A17&amp;"-compact"))</f>
-        <v>2</v>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A17)</f>
+        <v>4</v>
       </c>
       <c r="C17" s="3">
         <f>COUNTIF('epub-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A17,"-compact", ""),"-descriptive", ""))</f>
@@ -1504,11 +1505,11 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="str">
-        <v>conformance-epub-accessibility-1-1</v>
+        <v>conformance-certifier-credentials-prefix</v>
       </c>
       <c r="B18" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A18),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A18&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A18&amp;"-compact"))</f>
-        <v>1</v>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A18)</f>
+        <v>3</v>
       </c>
       <c r="C18" s="3">
         <f>COUNTIF('epub-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A18,"-compact", ""),"-descriptive", ""))</f>
@@ -1521,11 +1522,11 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="str">
-        <v>conformance-wcag-2-1</v>
+        <v>conformance-details</v>
       </c>
       <c r="B19" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A19),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A19&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A19&amp;"-compact"))</f>
-        <v>1</v>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A19)</f>
+        <v>2</v>
       </c>
       <c r="C19" s="3">
         <f>COUNTIF('epub-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A19,"-compact", ""),"-descriptive", ""))</f>
@@ -1538,11 +1539,11 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="str">
-        <v>conformance-level-aa</v>
+        <v>conformance-claim</v>
       </c>
       <c r="B20" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A20),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A20&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A20&amp;"-compact"))</f>
-        <v>1</v>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A20)</f>
+        <v>2</v>
       </c>
       <c r="C20" s="3">
         <f>COUNTIF('epub-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A20,"-compact", ""),"-descriptive", ""))</f>
@@ -1555,11 +1556,11 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="str">
-        <v>conformance-certification-date-prefix</v>
+        <v>conformance-epub-accessibility-1-1</v>
       </c>
       <c r="B21" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A21),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A21&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A21&amp;"-compact"))</f>
-        <v>2</v>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A21)</f>
+        <v>1</v>
       </c>
       <c r="C21" s="3">
         <f>COUNTIF('epub-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A21,"-compact", ""),"-descriptive", ""))</f>
@@ -1572,11 +1573,11 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="str">
-        <v>conformance-certifier-report</v>
+        <v>conformance-wcag-2-1</v>
       </c>
       <c r="B22" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A22),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A22&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A22&amp;"-compact"))</f>
-        <v>2</v>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A22)</f>
+        <v>1</v>
       </c>
       <c r="C22" s="3">
         <f>COUNTIF('epub-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A22,"-compact", ""),"-descriptive", ""))</f>
@@ -1589,10 +1590,10 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" t="str">
-        <v>conformance-a</v>
+        <v>conformance-level-aa</v>
       </c>
       <c r="B23" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A23),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A23&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A23&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A23)</f>
         <v>1</v>
       </c>
       <c r="C23" s="3">
@@ -1606,11 +1607,11 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" t="str">
-        <v>conformance-epub-accessibility-1-0</v>
+        <v>conformance-certification-date-prefix</v>
       </c>
       <c r="B24" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A24),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A24&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A24&amp;"-compact"))</f>
-        <v>1</v>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A24)</f>
+        <v>2</v>
       </c>
       <c r="C24" s="3">
         <f>COUNTIF('epub-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A24,"-compact", ""),"-descriptive", ""))</f>
@@ -1623,11 +1624,11 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" t="str">
-        <v>conformance-wcag-2-0</v>
+        <v>conformance-certifier-report</v>
       </c>
       <c r="B25" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A25),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A25&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A25&amp;"-compact"))</f>
-        <v>1</v>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A25)</f>
+        <v>2</v>
       </c>
       <c r="C25" s="3">
         <f>COUNTIF('epub-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A25,"-compact", ""),"-descriptive", ""))</f>
@@ -1640,10 +1641,10 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="str">
-        <v>conformance-level-a</v>
+        <v>conformance-epub-accessibility-1-0</v>
       </c>
       <c r="B26" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A26),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A26&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A26&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A26)</f>
         <v>1</v>
       </c>
       <c r="C26" s="3">
@@ -1657,28 +1658,28 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="str">
-        <v>pre-recorded-audio-title</v>
+        <v>conformance-wcag-2-0</v>
       </c>
       <c r="B27" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A27),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A27&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A27&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A27)</f>
         <v>1</v>
       </c>
       <c r="C27" s="3">
         <f>COUNTIF('epub-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A27,"-compact", ""),"-descriptive", ""))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D27" s="3">
         <f>COUNTIF('onix-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A27,"-compact", ""),"-descriptive", ""))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" t="str">
-        <v>pre-recorded-audio-only</v>
+        <v>conformance-level-a</v>
       </c>
       <c r="B28" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A28),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A28&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A28&amp;"-compact"))</f>
-        <v>2</v>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A28)</f>
+        <v>1</v>
       </c>
       <c r="C28" s="3">
         <f>COUNTIF('epub-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A28,"-compact", ""),"-descriptive", ""))</f>
@@ -1691,11 +1692,11 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="str">
-        <v>pre-recorded-audio-complementary</v>
+        <v>conformance-certifier</v>
       </c>
       <c r="B29" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A29),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A29&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A29&amp;"-compact"))</f>
-        <v>2</v>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A29)</f>
+        <v>1</v>
       </c>
       <c r="C29" s="3">
         <f>COUNTIF('epub-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A29,"-compact", ""),"-descriptive", ""))</f>
@@ -1708,11 +1709,11 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A30" t="str">
-        <v>pre-recorded-audio-synchronized</v>
+        <v>conformance-certifier-credentials</v>
       </c>
       <c r="B30" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A30),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A30&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A30&amp;"-compact"))</f>
-        <v>2</v>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A30)</f>
+        <v>1</v>
       </c>
       <c r="C30" s="3">
         <f>COUNTIF('epub-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A30,"-compact", ""),"-descriptive", ""))</f>
@@ -1725,10 +1726,10 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="str">
-        <v>navigation-title</v>
+        <v>pre-recorded-audio-title</v>
       </c>
       <c r="B31" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A31),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A31&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A31&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A31)</f>
         <v>1</v>
       </c>
       <c r="C31" s="3">
@@ -1742,10 +1743,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" t="str">
-        <v>navigation-toc</v>
+        <v>pre-recorded-audio-only</v>
       </c>
       <c r="B32" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A32),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A32&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A32&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A32)</f>
         <v>2</v>
       </c>
       <c r="C32" s="3">
@@ -1759,10 +1760,10 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="str">
-        <v>navigation-index</v>
+        <v>pre-recorded-audio-complementary</v>
       </c>
       <c r="B33" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A33),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A33&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A33&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A33)</f>
         <v>2</v>
       </c>
       <c r="C33" s="3">
@@ -1776,45 +1777,45 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" t="str">
-        <v>navigation-landmarks</v>
+        <v>pre-recorded-audio-synchronized</v>
       </c>
       <c r="B34" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A34),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A34&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A34&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A34)</f>
         <v>2</v>
       </c>
       <c r="C34" s="3">
         <f>COUNTIF('epub-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A34,"-compact", ""),"-descriptive", ""))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D34" s="3">
         <f>COUNTIF('onix-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A34,"-compact", ""),"-descriptive", ""))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A35" t="str">
-        <v>navigation-page-navigation</v>
+        <v>navigation-title</v>
       </c>
       <c r="B35" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A35),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A35&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A35&amp;"-compact"))</f>
-        <v>2</v>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A35)</f>
+        <v>1</v>
       </c>
       <c r="C35" s="3">
         <f>COUNTIF('epub-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A35,"-compact", ""),"-descriptive", ""))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D35" s="3">
         <f>COUNTIF('onix-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A35,"-compact", ""),"-descriptive", ""))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" t="str">
-        <v>navigation-intro</v>
+        <v>navigation-toc</v>
       </c>
       <c r="B36" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A36),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A36&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A36&amp;"-compact"))</f>
-        <v>1</v>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A36)</f>
+        <v>2</v>
       </c>
       <c r="C36" s="3">
         <f>COUNTIF('epub-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A36,"-compact", ""),"-descriptive", ""))</f>
@@ -1827,10 +1828,10 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A37" t="str">
-        <v>join-array-and</v>
+        <v>navigation-index</v>
       </c>
       <c r="B37" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A37),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A37&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A37&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A37)</f>
         <v>2</v>
       </c>
       <c r="C37" s="3">
@@ -1844,11 +1845,11 @@
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" t="str">
-        <v>charts-diagrams-formulas-title</v>
+        <v>navigation-landmarks</v>
       </c>
       <c r="B38" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A38),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A38&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A38&amp;"-compact"))</f>
-        <v>1</v>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A38)</f>
+        <v>2</v>
       </c>
       <c r="C38" s="3">
         <f>COUNTIF('epub-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A38,"-compact", ""),"-descriptive", ""))</f>
@@ -1861,10 +1862,10 @@
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" t="str">
-        <v>charts-diagrams-formulas-extended</v>
+        <v>navigation-page-navigation</v>
       </c>
       <c r="B39" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A39),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A39&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A39&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A39)</f>
         <v>2</v>
       </c>
       <c r="C39" s="3">
@@ -1878,11 +1879,11 @@
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" t="str">
-        <v>charts-diagrams-formulas-accessible-math</v>
+        <v>navigation-intro</v>
       </c>
       <c r="B40" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A40),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A40&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A40&amp;"-compact"))</f>
-        <v>2</v>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A40)</f>
+        <v>1</v>
       </c>
       <c r="C40" s="3">
         <f>COUNTIF('epub-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A40,"-compact", ""),"-descriptive", ""))</f>
@@ -1895,10 +1896,10 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="str">
-        <v>charts-diagrams-formulas-unknown</v>
+        <v>join-array-and</v>
       </c>
       <c r="B41" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A41),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A41&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A41&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A41)</f>
         <v>2</v>
       </c>
       <c r="C41" s="3">
@@ -1912,10 +1913,10 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" t="str">
-        <v>hazards-title</v>
+        <v>charts-diagrams-formulas-title</v>
       </c>
       <c r="B42" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A42),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A42&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A42&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A42)</f>
         <v>1</v>
       </c>
       <c r="C42" s="3">
@@ -1929,10 +1930,10 @@
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="str">
-        <v>hazards-none</v>
+        <v>charts-diagrams-formulas-extended</v>
       </c>
       <c r="B43" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A43),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A43&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A43&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A43)</f>
         <v>2</v>
       </c>
       <c r="C43" s="3">
@@ -1946,10 +1947,10 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="str">
-        <v>hazards-flashing</v>
+        <v>charts-diagrams-formulas-accessible-math</v>
       </c>
       <c r="B44" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A44),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A44&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A44&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A44)</f>
         <v>2</v>
       </c>
       <c r="C44" s="3">
@@ -1963,11 +1964,11 @@
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A45" t="str">
-        <v>hazards-sound</v>
+        <v>charts-diagrams-formulas-unknown</v>
       </c>
       <c r="B45" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A45),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A45&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A45&amp;"-compact"))</f>
-        <v>1</v>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A45)</f>
+        <v>2</v>
       </c>
       <c r="C45" s="3">
         <f>COUNTIF('epub-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A45,"-compact", ""),"-descriptive", ""))</f>
@@ -1980,44 +1981,44 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="str">
-        <v>hazards-motion</v>
+        <v>hazards-title</v>
       </c>
       <c r="B46" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A46),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A46&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A46&amp;"-compact"))</f>
-        <v>2</v>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A46)</f>
+        <v>1</v>
       </c>
       <c r="C46" s="3">
         <f>COUNTIF('epub-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A46,"-compact", ""),"-descriptive", ""))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D46" s="3">
         <f>COUNTIF('onix-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A46,"-compact", ""),"-descriptive", ""))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" t="str">
-        <v>hasards-explanatory</v>
+        <v>hazards-none</v>
       </c>
       <c r="B47" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A47),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A47&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A47&amp;"-compact"))</f>
-        <v>1</v>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A47)</f>
+        <v>2</v>
       </c>
       <c r="C47" s="3">
         <f>COUNTIF('epub-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A47,"-compact", ""),"-descriptive", ""))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D47" s="3">
         <f>COUNTIF('onix-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A47,"-compact", ""),"-descriptive", ""))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" t="str">
-        <v>hazards-unknown</v>
+        <v>hazards-flashing</v>
       </c>
       <c r="B48" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A48),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A48&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A48&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A48)</f>
         <v>2</v>
       </c>
       <c r="C48" s="3">
@@ -2031,62 +2032,62 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" t="str">
-        <v>accessibility-summary-title</v>
+        <v>hazards-sound</v>
       </c>
       <c r="B49" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A49),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A49&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A49&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A49)</f>
         <v>1</v>
       </c>
       <c r="C49" s="3">
         <f>COUNTIF('epub-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A49,"-compact", ""),"-descriptive", ""))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D49" s="3">
         <f>COUNTIF('onix-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A49,"-compact", ""),"-descriptive", ""))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" t="str">
-        <v>additional-accessibility-information-title</v>
+        <v>hazards-motion</v>
       </c>
       <c r="B50" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A50),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A50&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A50&amp;"-compact"))</f>
-        <v>1</v>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A50)</f>
+        <v>2</v>
       </c>
       <c r="C50" s="3">
         <f>COUNTIF('epub-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A50,"-compact", ""),"-descriptive", ""))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D50" s="3">
         <f>COUNTIF('onix-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A50,"-compact", ""),"-descriptive", ""))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" t="str">
-        <v>conformance-aaa</v>
+        <v>hasards-explanatory</v>
       </c>
       <c r="B51" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A51),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A51&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A51&amp;"-compact"))</f>
-        <v>0</v>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A51)</f>
+        <v>1</v>
       </c>
       <c r="C51" s="3">
         <f>COUNTIF('epub-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A51,"-compact", ""),"-descriptive", ""))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D51" s="3">
         <f>COUNTIF('onix-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A51,"-compact", ""),"-descriptive", ""))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" t="str">
-        <v>unknown-conformance</v>
+        <v>hazards-unknown</v>
       </c>
       <c r="B52" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A52),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A52&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A52&amp;"-compact"))</f>
-        <v>0</v>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A52)</f>
+        <v>2</v>
       </c>
       <c r="C52" s="3">
         <f>COUNTIF('epub-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A52,"-compact", ""),"-descriptive", ""))</f>
@@ -2094,49 +2095,49 @@
       </c>
       <c r="D52" s="3">
         <f>COUNTIF('onix-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A52,"-compact", ""),"-descriptive", ""))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" t="str">
-        <v>conformance-no</v>
+        <v>accessibility-summary-title</v>
       </c>
       <c r="B53" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A53),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A53&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A53&amp;"-compact"))</f>
-        <v>0</v>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A53)</f>
+        <v>1</v>
       </c>
       <c r="C53" s="3">
         <f>COUNTIF('epub-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A53,"-compact", ""),"-descriptive", ""))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D53" s="3">
         <f>COUNTIF('onix-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A53,"-compact", ""),"-descriptive", ""))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A54" t="str">
-        <v>conformance-certifier</v>
+        <v>additional-accessibility-information-title</v>
       </c>
       <c r="B54" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A54),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A54&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A54&amp;"-compact"))</f>
-        <v>0</v>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A54)</f>
+        <v>1</v>
       </c>
       <c r="C54" s="3">
         <f>COUNTIF('epub-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A54,"-compact", ""),"-descriptive", ""))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D54" s="3">
         <f>COUNTIF('onix-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A54,"-compact", ""),"-descriptive", ""))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" t="str">
-        <v>conformance-certifier-credentials</v>
+        <v>unknown-conformance</v>
       </c>
       <c r="B55" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A55),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A55&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A55&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A55)</f>
         <v>0</v>
       </c>
       <c r="C55" s="3">
@@ -2145,7 +2146,7 @@
       </c>
       <c r="D55" s="3">
         <f>COUNTIF('onix-metadata-strings'!$D$2:$D$67,SUBSTITUTE(SUBSTITUTE(crosscheck!$A55,"-compact", ""),"-descriptive", ""))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -2153,7 +2154,7 @@
         <v>conformance-wcag-2-2</v>
       </c>
       <c r="B56" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A56),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A56&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A56&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A56)</f>
         <v>0</v>
       </c>
       <c r="C56" s="3">
@@ -2170,7 +2171,7 @@
         <v>conformance-level-aaa</v>
       </c>
       <c r="B57" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A57),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A57&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A57&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A57)</f>
         <v>0</v>
       </c>
       <c r="C57" s="3">
@@ -2187,7 +2188,7 @@
         <v>pre-recorded-audio-no-metadata</v>
       </c>
       <c r="B58" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A58),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A58&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A58&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A58)</f>
         <v>0</v>
       </c>
       <c r="C58" s="3">
@@ -2204,7 +2205,7 @@
         <v>navigation-structural</v>
       </c>
       <c r="B59" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A59),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A59&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A59&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A59)</f>
         <v>0</v>
       </c>
       <c r="C59" s="3">
@@ -2221,7 +2222,7 @@
         <v>navigation-no-metadata</v>
       </c>
       <c r="B60" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A60),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A60&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A60&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A60)</f>
         <v>0</v>
       </c>
       <c r="C60" s="3">
@@ -2238,7 +2239,7 @@
         <v>charts-diagrams-formulas-accessible-chemistry</v>
       </c>
       <c r="B61" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A61),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A61&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A61&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A61)</f>
         <v>0</v>
       </c>
       <c r="C61" s="3">
@@ -2255,7 +2256,7 @@
         <v>hazards-plural</v>
       </c>
       <c r="B62" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A62),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A62&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A62&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A62)</f>
         <v>0</v>
       </c>
       <c r="C62" s="3">
@@ -2272,7 +2273,7 @@
         <v>hazards-singular</v>
       </c>
       <c r="B63" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A63),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A63&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A63&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A63)</f>
         <v>0</v>
       </c>
       <c r="C63" s="3">
@@ -2289,7 +2290,7 @@
         <v>hazards-no-metadata</v>
       </c>
       <c r="B64" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A64),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A64&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A64&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A64)</f>
         <v>0</v>
       </c>
       <c r="C64" s="3">
@@ -2306,7 +2307,7 @@
         <v>accessibility-summary-no-metadata</v>
       </c>
       <c r="B65" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A65),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A65&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A65&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A65)</f>
         <v>0</v>
       </c>
       <c r="C65" s="3">
@@ -2323,7 +2324,7 @@
         <v>tbd</v>
       </c>
       <c r="B66" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A66),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A66&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A66&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A66)</f>
         <v>0</v>
       </c>
       <c r="C66" s="3">
@@ -2340,7 +2341,7 @@
         <v>legal-considerations-no-metadata</v>
       </c>
       <c r="B67" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A67),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A67&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A67&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A67)</f>
         <v>0</v>
       </c>
       <c r="C67" s="3">
@@ -2357,7 +2358,7 @@
         <v>additional-accessibility-information-adaptation-audio-descriptions</v>
       </c>
       <c r="B68" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A68),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A68&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A68&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A68)</f>
         <v>0</v>
       </c>
       <c r="C68" s="3">
@@ -2374,7 +2375,7 @@
         <v>additional-accessibility-information-adaptation-braille</v>
       </c>
       <c r="B69" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A69),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A69&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A69&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A69)</f>
         <v>0</v>
       </c>
       <c r="C69" s="3">
@@ -2391,7 +2392,7 @@
         <v>additional-accessibility-information-adaptation-closed-captions</v>
       </c>
       <c r="B70" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A70),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A70&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A70&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A70)</f>
         <v>0</v>
       </c>
       <c r="C70" s="3">
@@ -2408,7 +2409,7 @@
         <v>additional-accessibility-information-adaptation-open-captions</v>
       </c>
       <c r="B71" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A71),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A71&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A71&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A71)</f>
         <v>0</v>
       </c>
       <c r="C71" s="3">
@@ -2425,7 +2426,7 @@
         <v>additional-accessibility-information-adaptation-tactile_graphic</v>
       </c>
       <c r="B72" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A72),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A72&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A72&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A72)</f>
         <v>0</v>
       </c>
       <c r="C72" s="3">
@@ -2442,7 +2443,7 @@
         <v>additional-accessibility-information-adaptation-tactile_object</v>
       </c>
       <c r="B73" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A73),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A73&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A73&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A73)</f>
         <v>0</v>
       </c>
       <c r="C73" s="3">
@@ -2459,7 +2460,7 @@
         <v>additional-accessibility-information-adaptation-transcript</v>
       </c>
       <c r="B74" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A74),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A74&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A74&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A74)</f>
         <v>0</v>
       </c>
       <c r="C74" s="3">
@@ -2476,7 +2477,7 @@
         <v>additional-accessibility-information-adaptation-sign-language</v>
       </c>
       <c r="B75" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A75),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A75&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A75&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A75)</f>
         <v>0</v>
       </c>
       <c r="C75" s="3">
@@ -2493,7 +2494,7 @@
         <v>additional-accessibility-information-clarity-aria</v>
       </c>
       <c r="B76" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A76),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A76&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A76&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A76)</f>
         <v>0</v>
       </c>
       <c r="C76" s="3">
@@ -2510,7 +2511,7 @@
         <v>additional-accessibility-information-clarity-full-ruby-annotations</v>
       </c>
       <c r="B77" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A77),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A77&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A77&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A77)</f>
         <v>0</v>
       </c>
       <c r="C77" s="3">
@@ -2527,7 +2528,7 @@
         <v>additional-accessibility-information-clarity-text-to-speech-hinting</v>
       </c>
       <c r="B78" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A78),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A78&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A78&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A78)</f>
         <v>0</v>
       </c>
       <c r="C78" s="3">
@@ -2544,7 +2545,7 @@
         <v>additional-accessibility-information-clarity-high-contrast-between-foreground-and-background-audio</v>
       </c>
       <c r="B79" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A79),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A79&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A79&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A79)</f>
         <v>0</v>
       </c>
       <c r="C79" s="3">
@@ -2561,7 +2562,7 @@
         <v>additional-accessibility-information-clarity-high-contrast-between-text-and-background</v>
       </c>
       <c r="B80" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A80),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A80&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A80&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A80)</f>
         <v>0</v>
       </c>
       <c r="C80" s="3">
@@ -2578,7 +2579,7 @@
         <v>additional-accessibility-information-clarity-large-print</v>
       </c>
       <c r="B81" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A81),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A81&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A81&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A81)</f>
         <v>0</v>
       </c>
       <c r="C81" s="3">
@@ -2595,7 +2596,7 @@
         <v>additional-accessibility-information-clarity-page-breaks</v>
       </c>
       <c r="B82" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A82),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A82&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A82&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A82)</f>
         <v>0</v>
       </c>
       <c r="C82" s="3">
@@ -2612,7 +2613,7 @@
         <v>additional-accessibility-information-clarity-ruby-annotations</v>
       </c>
       <c r="B83" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A83),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A83&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A83&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A83)</f>
         <v>0</v>
       </c>
       <c r="C83" s="3">
@@ -2629,7 +2630,7 @@
         <v>charts-diagrams-formulas-non-graphical-data</v>
       </c>
       <c r="B84" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A84),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A84&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A84&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A84)</f>
         <v>0</v>
       </c>
       <c r="C84" s="3">
@@ -2646,7 +2647,7 @@
         <v>additional-accessibility-information-adaptation-dyslexia-readability</v>
       </c>
       <c r="B85" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A85),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A85&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A85&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A85)</f>
         <v>0</v>
       </c>
       <c r="C85" s="3">
@@ -2663,7 +2664,7 @@
         <v>additional-accessibility-information-adaptation-full-transcript</v>
       </c>
       <c r="B86" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A86),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A86&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A86&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A86)</f>
         <v>0</v>
       </c>
       <c r="C86" s="3">
@@ -2680,7 +2681,7 @@
         <v>additional-accessibility-information-clarity-color-not-sole-means-of-conveying-information</v>
       </c>
       <c r="B87" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A87),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A87&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A87&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A87)</f>
         <v>0</v>
       </c>
       <c r="C87" s="3">
@@ -2697,7 +2698,7 @@
         <v>additional-accessibility-information-clarity-ultra-high-contrast-between-text-and-background</v>
       </c>
       <c r="B88" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A88),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A88&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A88&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A88)</f>
         <v>0</v>
       </c>
       <c r="C88" s="3">
@@ -2714,7 +2715,7 @@
         <v>additional-accessibility-information-clarity-visible-page-numbering</v>
       </c>
       <c r="B89" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A89),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A89&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A89&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A89)</f>
         <v>0</v>
       </c>
       <c r="C89" s="3">
@@ -2731,7 +2732,7 @@
         <v>additional-accessibility-information-clarity-without-background-sounds</v>
       </c>
       <c r="B90" s="3">
-        <f>MAX(COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A90),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A90&amp;"-descriptive"),COUNTIF('principles-string'!$D$2:$D$84,crosscheck!$A90&amp;"-compact"))</f>
+        <f>COUNTIF('principles-string'!$D$2:$D$94,crosscheck!$A90)</f>
         <v>0</v>
       </c>
       <c r="C90" s="3">
@@ -3079,11 +3080,12 @@
       <c r="D157" s="3"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D90" xr:uid="{3A9EDDE9-AF31-2D43-AC52-4CD1D03679BB}"/>
   <conditionalFormatting sqref="B2:D90">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3093,10 +3095,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DAAE526-051A-2147-9F70-F78890C8D07D}">
-  <dimension ref="A1:F84"/>
+  <dimension ref="A1:F94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F84"/>
+      <selection sqref="A1:F94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3359,13 +3361,13 @@
         <v>148</v>
       </c>
       <c r="D19" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E19" t="s">
         <v>230</v>
       </c>
       <c r="F19" t="s">
-        <v>189</v>
+        <v>238</v>
       </c>
     </row>
     <row r="20" spans="3:6" x14ac:dyDescent="0.2">
@@ -3373,13 +3375,13 @@
         <v>148</v>
       </c>
       <c r="D20" t="s">
-        <v>43</v>
+        <v>9</v>
       </c>
       <c r="E20" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F20" t="s">
-        <v>44</v>
+        <v>239</v>
       </c>
     </row>
     <row r="21" spans="3:6" x14ac:dyDescent="0.2">
@@ -3387,13 +3389,13 @@
         <v>148</v>
       </c>
       <c r="D21" t="s">
-        <v>46</v>
+        <v>11</v>
       </c>
       <c r="E21" t="s">
         <v>230</v>
       </c>
       <c r="F21" t="s">
-        <v>47</v>
+        <v>189</v>
       </c>
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.2">
@@ -3401,13 +3403,13 @@
         <v>148</v>
       </c>
       <c r="D22" t="s">
-        <v>48</v>
+        <v>11</v>
       </c>
       <c r="E22" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F22" t="s">
-        <v>22</v>
+        <v>240</v>
       </c>
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.2">
@@ -3415,10 +3417,13 @@
         <v>148</v>
       </c>
       <c r="D23" t="s">
-        <v>23</v>
+        <v>13</v>
+      </c>
+      <c r="E23" t="s">
+        <v>230</v>
       </c>
       <c r="F23" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
     </row>
     <row r="24" spans="3:6" x14ac:dyDescent="0.2">
@@ -3426,10 +3431,13 @@
         <v>148</v>
       </c>
       <c r="D24" t="s">
-        <v>25</v>
+        <v>13</v>
+      </c>
+      <c r="E24" t="s">
+        <v>227</v>
       </c>
       <c r="F24" t="s">
-        <v>26</v>
+        <v>241</v>
       </c>
     </row>
     <row r="25" spans="3:6" x14ac:dyDescent="0.2">
@@ -3437,10 +3445,13 @@
         <v>148</v>
       </c>
       <c r="D25" t="s">
-        <v>29</v>
+        <v>17</v>
+      </c>
+      <c r="E25" t="s">
+        <v>230</v>
       </c>
       <c r="F25" t="s">
-        <v>30</v>
+        <v>242</v>
       </c>
     </row>
     <row r="26" spans="3:6" x14ac:dyDescent="0.2">
@@ -3448,13 +3459,13 @@
         <v>148</v>
       </c>
       <c r="D26" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="E26" t="s">
         <v>227</v>
       </c>
       <c r="F26" t="s">
-        <v>191</v>
+        <v>243</v>
       </c>
     </row>
     <row r="27" spans="3:6" x14ac:dyDescent="0.2">
@@ -3462,10 +3473,13 @@
         <v>148</v>
       </c>
       <c r="D27" t="s">
-        <v>39</v>
+        <v>11</v>
+      </c>
+      <c r="E27" t="s">
+        <v>230</v>
       </c>
       <c r="F27" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="28" spans="3:6" x14ac:dyDescent="0.2">
@@ -3476,7 +3490,7 @@
         <v>43</v>
       </c>
       <c r="E28" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="F28" t="s">
         <v>44</v>
@@ -3487,10 +3501,13 @@
         <v>148</v>
       </c>
       <c r="D29" t="s">
-        <v>152</v>
+        <v>46</v>
+      </c>
+      <c r="E29" t="s">
+        <v>230</v>
       </c>
       <c r="F29" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
     </row>
     <row r="30" spans="3:6" x14ac:dyDescent="0.2">
@@ -3498,13 +3515,13 @@
         <v>148</v>
       </c>
       <c r="D30" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E30" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="F30" t="s">
-        <v>47</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="3:6" x14ac:dyDescent="0.2">
@@ -3512,10 +3529,10 @@
         <v>148</v>
       </c>
       <c r="D31" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="F31" t="s">
-        <v>49</v>
+        <v>190</v>
       </c>
     </row>
     <row r="32" spans="3:6" x14ac:dyDescent="0.2">
@@ -3523,10 +3540,10 @@
         <v>148</v>
       </c>
       <c r="D32" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="F32" t="s">
-        <v>234</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="3:6" x14ac:dyDescent="0.2">
@@ -3534,13 +3551,10 @@
         <v>148</v>
       </c>
       <c r="D33" t="s">
-        <v>13</v>
-      </c>
-      <c r="E33" t="s">
-        <v>230</v>
+        <v>29</v>
       </c>
       <c r="F33" t="s">
-        <v>193</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="3:6" x14ac:dyDescent="0.2">
@@ -3548,13 +3562,13 @@
         <v>148</v>
       </c>
       <c r="D34" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="E34" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F34" t="s">
-        <v>44</v>
+        <v>191</v>
       </c>
     </row>
     <row r="35" spans="3:6" x14ac:dyDescent="0.2">
@@ -3562,13 +3576,10 @@
         <v>148</v>
       </c>
       <c r="D35" t="s">
-        <v>46</v>
-      </c>
-      <c r="E35" t="s">
-        <v>230</v>
+        <v>39</v>
       </c>
       <c r="F35" t="s">
-        <v>47</v>
+        <v>192</v>
       </c>
     </row>
     <row r="36" spans="3:6" x14ac:dyDescent="0.2">
@@ -3576,10 +3587,13 @@
         <v>148</v>
       </c>
       <c r="D36" t="s">
-        <v>23</v>
+        <v>43</v>
+      </c>
+      <c r="E36" t="s">
+        <v>227</v>
       </c>
       <c r="F36" t="s">
-        <v>190</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37" spans="3:6" x14ac:dyDescent="0.2">
@@ -3587,10 +3601,10 @@
         <v>148</v>
       </c>
       <c r="D37" t="s">
-        <v>25</v>
+        <v>152</v>
       </c>
       <c r="F37" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
     </row>
     <row r="38" spans="3:6" x14ac:dyDescent="0.2">
@@ -3598,10 +3612,13 @@
         <v>148</v>
       </c>
       <c r="D38" t="s">
-        <v>27</v>
+        <v>46</v>
+      </c>
+      <c r="E38" t="s">
+        <v>227</v>
       </c>
       <c r="F38" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
     </row>
     <row r="39" spans="3:6" x14ac:dyDescent="0.2">
@@ -3609,13 +3626,10 @@
         <v>148</v>
       </c>
       <c r="D39" t="s">
-        <v>31</v>
-      </c>
-      <c r="E39" t="s">
-        <v>227</v>
+        <v>48</v>
       </c>
       <c r="F39" t="s">
-        <v>194</v>
+        <v>49</v>
       </c>
     </row>
     <row r="40" spans="3:6" x14ac:dyDescent="0.2">
@@ -3623,10 +3637,10 @@
         <v>148</v>
       </c>
       <c r="D40" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="F40" t="s">
-        <v>195</v>
+        <v>234</v>
       </c>
     </row>
     <row r="41" spans="3:6" x14ac:dyDescent="0.2">
@@ -3634,13 +3648,13 @@
         <v>148</v>
       </c>
       <c r="D41" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="E41" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="F41" t="s">
-        <v>44</v>
+        <v>193</v>
       </c>
     </row>
     <row r="42" spans="3:6" x14ac:dyDescent="0.2">
@@ -3648,10 +3662,13 @@
         <v>148</v>
       </c>
       <c r="D42" t="s">
-        <v>152</v>
+        <v>43</v>
+      </c>
+      <c r="E42" t="s">
+        <v>230</v>
       </c>
       <c r="F42" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="43" spans="3:6" x14ac:dyDescent="0.2">
@@ -3662,7 +3679,7 @@
         <v>46</v>
       </c>
       <c r="E43" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="F43" t="s">
         <v>47</v>
@@ -3673,10 +3690,10 @@
         <v>148</v>
       </c>
       <c r="D44" t="s">
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="F44" t="s">
-        <v>49</v>
+        <v>190</v>
       </c>
     </row>
     <row r="45" spans="3:6" x14ac:dyDescent="0.2">
@@ -3684,10 +3701,10 @@
         <v>148</v>
       </c>
       <c r="D45" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="F45" t="s">
-        <v>234</v>
+        <v>26</v>
       </c>
     </row>
     <row r="46" spans="3:6" x14ac:dyDescent="0.2">
@@ -3695,10 +3712,10 @@
         <v>148</v>
       </c>
       <c r="D46" t="s">
-        <v>170</v>
+        <v>27</v>
       </c>
       <c r="F46" t="s">
-        <v>171</v>
+        <v>28</v>
       </c>
     </row>
     <row r="47" spans="3:6" x14ac:dyDescent="0.2">
@@ -3706,13 +3723,13 @@
         <v>148</v>
       </c>
       <c r="D47" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="E47" t="s">
         <v>227</v>
       </c>
       <c r="F47" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="48" spans="3:6" x14ac:dyDescent="0.2">
@@ -3720,13 +3737,10 @@
         <v>148</v>
       </c>
       <c r="D48" t="s">
-        <v>56</v>
-      </c>
-      <c r="E48" t="s">
-        <v>227</v>
+        <v>41</v>
       </c>
       <c r="F48" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="49" spans="3:6" x14ac:dyDescent="0.2">
@@ -3734,13 +3748,13 @@
         <v>148</v>
       </c>
       <c r="D49" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="E49" t="s">
         <v>227</v>
       </c>
       <c r="F49" t="s">
-        <v>198</v>
+        <v>44</v>
       </c>
     </row>
     <row r="50" spans="3:6" x14ac:dyDescent="0.2">
@@ -3748,13 +3762,10 @@
         <v>148</v>
       </c>
       <c r="D50" t="s">
-        <v>52</v>
-      </c>
-      <c r="E50" t="s">
-        <v>230</v>
+        <v>152</v>
       </c>
       <c r="F50" t="s">
-        <v>199</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51" spans="3:6" x14ac:dyDescent="0.2">
@@ -3762,13 +3773,13 @@
         <v>148</v>
       </c>
       <c r="D51" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="E51" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F51" t="s">
-        <v>200</v>
+        <v>47</v>
       </c>
     </row>
     <row r="52" spans="3:6" x14ac:dyDescent="0.2">
@@ -3776,13 +3787,10 @@
         <v>148</v>
       </c>
       <c r="D52" t="s">
-        <v>54</v>
-      </c>
-      <c r="E52" t="s">
-        <v>230</v>
+        <v>48</v>
       </c>
       <c r="F52" t="s">
-        <v>201</v>
+        <v>49</v>
       </c>
     </row>
     <row r="53" spans="3:6" x14ac:dyDescent="0.2">
@@ -3790,10 +3798,10 @@
         <v>148</v>
       </c>
       <c r="D53" t="s">
-        <v>172</v>
+        <v>50</v>
       </c>
       <c r="F53" t="s">
-        <v>173</v>
+        <v>234</v>
       </c>
     </row>
     <row r="54" spans="3:6" x14ac:dyDescent="0.2">
@@ -3801,13 +3809,10 @@
         <v>148</v>
       </c>
       <c r="D54" t="s">
-        <v>60</v>
-      </c>
-      <c r="E54" t="s">
-        <v>227</v>
+        <v>19</v>
       </c>
       <c r="F54" t="s">
-        <v>202</v>
+        <v>20</v>
       </c>
     </row>
     <row r="55" spans="3:6" x14ac:dyDescent="0.2">
@@ -3815,13 +3820,10 @@
         <v>148</v>
       </c>
       <c r="D55" t="s">
-        <v>62</v>
-      </c>
-      <c r="E55" t="s">
-        <v>227</v>
+        <v>21</v>
       </c>
       <c r="F55" t="s">
-        <v>203</v>
+        <v>22</v>
       </c>
     </row>
     <row r="56" spans="3:6" x14ac:dyDescent="0.2">
@@ -3829,13 +3831,10 @@
         <v>148</v>
       </c>
       <c r="D56" t="s">
-        <v>235</v>
-      </c>
-      <c r="E56" t="s">
-        <v>227</v>
+        <v>170</v>
       </c>
       <c r="F56" t="s">
-        <v>204</v>
+        <v>171</v>
       </c>
     </row>
     <row r="57" spans="3:6" x14ac:dyDescent="0.2">
@@ -3843,13 +3842,13 @@
         <v>148</v>
       </c>
       <c r="D57" t="s">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="E57" t="s">
         <v>227</v>
       </c>
       <c r="F57" t="s">
-        <v>236</v>
+        <v>196</v>
       </c>
     </row>
     <row r="58" spans="3:6" x14ac:dyDescent="0.2">
@@ -3857,13 +3856,13 @@
         <v>148</v>
       </c>
       <c r="D58" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="E58" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F58" t="s">
-        <v>70</v>
+        <v>197</v>
       </c>
     </row>
     <row r="59" spans="3:6" x14ac:dyDescent="0.2">
@@ -3871,13 +3870,13 @@
         <v>148</v>
       </c>
       <c r="D59" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E59" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F59" t="s">
-        <v>61</v>
+        <v>198</v>
       </c>
     </row>
     <row r="60" spans="3:6" x14ac:dyDescent="0.2">
@@ -3885,13 +3884,13 @@
         <v>148</v>
       </c>
       <c r="D60" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="E60" t="s">
         <v>230</v>
       </c>
       <c r="F60" t="s">
-        <v>63</v>
+        <v>199</v>
       </c>
     </row>
     <row r="61" spans="3:6" x14ac:dyDescent="0.2">
@@ -3899,13 +3898,13 @@
         <v>148</v>
       </c>
       <c r="D61" t="s">
-        <v>235</v>
+        <v>56</v>
       </c>
       <c r="E61" t="s">
         <v>230</v>
       </c>
       <c r="F61" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="62" spans="3:6" x14ac:dyDescent="0.2">
@@ -3913,10 +3912,13 @@
         <v>148</v>
       </c>
       <c r="D62" t="s">
-        <v>68</v>
+        <v>54</v>
+      </c>
+      <c r="E62" t="s">
+        <v>230</v>
       </c>
       <c r="F62" t="s">
-        <v>124</v>
+        <v>201</v>
       </c>
     </row>
     <row r="63" spans="3:6" x14ac:dyDescent="0.2">
@@ -3924,13 +3926,10 @@
         <v>148</v>
       </c>
       <c r="D63" t="s">
-        <v>65</v>
-      </c>
-      <c r="E63" t="s">
-        <v>230</v>
+        <v>172</v>
       </c>
       <c r="F63" t="s">
-        <v>206</v>
+        <v>173</v>
       </c>
     </row>
     <row r="64" spans="3:6" x14ac:dyDescent="0.2">
@@ -3938,10 +3937,13 @@
         <v>148</v>
       </c>
       <c r="D64" t="s">
-        <v>174</v>
+        <v>60</v>
+      </c>
+      <c r="E64" t="s">
+        <v>227</v>
       </c>
       <c r="F64" t="s">
-        <v>175</v>
+        <v>202</v>
       </c>
     </row>
     <row r="65" spans="3:6" x14ac:dyDescent="0.2">
@@ -3949,13 +3951,13 @@
         <v>148</v>
       </c>
       <c r="D65" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="E65" t="s">
         <v>227</v>
       </c>
       <c r="F65" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
     </row>
     <row r="66" spans="3:6" x14ac:dyDescent="0.2">
@@ -3963,13 +3965,13 @@
         <v>148</v>
       </c>
       <c r="D66" t="s">
-        <v>77</v>
+        <v>235</v>
       </c>
       <c r="E66" t="s">
         <v>227</v>
       </c>
       <c r="F66" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
     </row>
     <row r="67" spans="3:6" x14ac:dyDescent="0.2">
@@ -3977,13 +3979,13 @@
         <v>148</v>
       </c>
       <c r="D67" t="s">
-        <v>140</v>
+        <v>65</v>
       </c>
       <c r="E67" t="s">
         <v>227</v>
       </c>
       <c r="F67" t="s">
-        <v>209</v>
+        <v>236</v>
       </c>
     </row>
     <row r="68" spans="3:6" x14ac:dyDescent="0.2">
@@ -3991,13 +3993,13 @@
         <v>148</v>
       </c>
       <c r="D68" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E68" t="s">
         <v>230</v>
       </c>
       <c r="F68" t="s">
-        <v>210</v>
+        <v>70</v>
       </c>
     </row>
     <row r="69" spans="3:6" x14ac:dyDescent="0.2">
@@ -4005,13 +4007,13 @@
         <v>148</v>
       </c>
       <c r="D69" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="E69" t="s">
         <v>230</v>
       </c>
       <c r="F69" t="s">
-        <v>211</v>
+        <v>61</v>
       </c>
     </row>
     <row r="70" spans="3:6" x14ac:dyDescent="0.2">
@@ -4019,13 +4021,13 @@
         <v>148</v>
       </c>
       <c r="D70" t="s">
-        <v>140</v>
+        <v>62</v>
       </c>
       <c r="E70" t="s">
         <v>230</v>
       </c>
       <c r="F70" t="s">
-        <v>212</v>
+        <v>63</v>
       </c>
     </row>
     <row r="71" spans="3:6" x14ac:dyDescent="0.2">
@@ -4033,10 +4035,13 @@
         <v>148</v>
       </c>
       <c r="D71" t="s">
-        <v>176</v>
+        <v>235</v>
+      </c>
+      <c r="E71" t="s">
+        <v>230</v>
       </c>
       <c r="F71" t="s">
-        <v>177</v>
+        <v>205</v>
       </c>
     </row>
     <row r="72" spans="3:6" x14ac:dyDescent="0.2">
@@ -4044,13 +4049,10 @@
         <v>148</v>
       </c>
       <c r="D72" t="s">
-        <v>80</v>
-      </c>
-      <c r="E72" t="s">
-        <v>227</v>
+        <v>68</v>
       </c>
       <c r="F72" t="s">
-        <v>213</v>
+        <v>124</v>
       </c>
     </row>
     <row r="73" spans="3:6" x14ac:dyDescent="0.2">
@@ -4058,13 +4060,13 @@
         <v>148</v>
       </c>
       <c r="D73" t="s">
-        <v>82</v>
+        <v>65</v>
       </c>
       <c r="E73" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="F73" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
     </row>
     <row r="74" spans="3:6" x14ac:dyDescent="0.2">
@@ -4072,13 +4074,10 @@
         <v>148</v>
       </c>
       <c r="D74" t="s">
-        <v>86</v>
-      </c>
-      <c r="E74" t="s">
-        <v>227</v>
+        <v>174</v>
       </c>
       <c r="F74" t="s">
-        <v>215</v>
+        <v>175</v>
       </c>
     </row>
     <row r="75" spans="3:6" x14ac:dyDescent="0.2">
@@ -4086,13 +4085,13 @@
         <v>148</v>
       </c>
       <c r="D75" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="E75" t="s">
         <v>227</v>
       </c>
       <c r="F75" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
     </row>
     <row r="76" spans="3:6" x14ac:dyDescent="0.2">
@@ -4100,13 +4099,13 @@
         <v>148</v>
       </c>
       <c r="D76" t="s">
-        <v>237</v>
+        <v>77</v>
       </c>
       <c r="E76" t="s">
         <v>227</v>
       </c>
       <c r="F76" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
     </row>
     <row r="77" spans="3:6" x14ac:dyDescent="0.2">
@@ -4114,13 +4113,13 @@
         <v>148</v>
       </c>
       <c r="D77" t="s">
-        <v>92</v>
+        <v>140</v>
       </c>
       <c r="E77" t="s">
         <v>227</v>
       </c>
       <c r="F77" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
     </row>
     <row r="78" spans="3:6" x14ac:dyDescent="0.2">
@@ -4128,24 +4127,27 @@
         <v>148</v>
       </c>
       <c r="D78" t="s">
-        <v>80</v>
+        <v>73</v>
       </c>
       <c r="E78" t="s">
         <v>230</v>
       </c>
+      <c r="F78" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="79" spans="3:6" x14ac:dyDescent="0.2">
       <c r="C79" t="s">
         <v>148</v>
       </c>
       <c r="D79" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E79" t="s">
         <v>230</v>
       </c>
       <c r="F79" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
     </row>
     <row r="80" spans="3:6" x14ac:dyDescent="0.2">
@@ -4153,10 +4155,13 @@
         <v>148</v>
       </c>
       <c r="D80" t="s">
-        <v>68</v>
+        <v>140</v>
+      </c>
+      <c r="E80" t="s">
+        <v>230</v>
       </c>
       <c r="F80" t="s">
-        <v>124</v>
+        <v>212</v>
       </c>
     </row>
     <row r="81" spans="3:6" x14ac:dyDescent="0.2">
@@ -4164,13 +4169,10 @@
         <v>148</v>
       </c>
       <c r="D81" t="s">
-        <v>84</v>
-      </c>
-      <c r="E81" t="s">
-        <v>230</v>
+        <v>176</v>
       </c>
       <c r="F81" t="s">
-        <v>220</v>
+        <v>177</v>
       </c>
     </row>
     <row r="82" spans="3:6" x14ac:dyDescent="0.2">
@@ -4178,13 +4180,13 @@
         <v>148</v>
       </c>
       <c r="D82" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="E82" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="F82" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
     </row>
     <row r="83" spans="3:6" x14ac:dyDescent="0.2">
@@ -4192,10 +4194,13 @@
         <v>148</v>
       </c>
       <c r="D83" t="s">
-        <v>178</v>
+        <v>82</v>
+      </c>
+      <c r="E83" t="s">
+        <v>227</v>
       </c>
       <c r="F83" t="s">
-        <v>179</v>
+        <v>214</v>
       </c>
     </row>
     <row r="84" spans="3:6" x14ac:dyDescent="0.2">
@@ -4203,9 +4208,140 @@
         <v>148</v>
       </c>
       <c r="D84" t="s">
+        <v>86</v>
+      </c>
+      <c r="E84" t="s">
+        <v>227</v>
+      </c>
+      <c r="F84" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="85" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C85" t="s">
+        <v>148</v>
+      </c>
+      <c r="D85" t="s">
+        <v>84</v>
+      </c>
+      <c r="E85" t="s">
+        <v>227</v>
+      </c>
+      <c r="F85" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="86" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C86" t="s">
+        <v>148</v>
+      </c>
+      <c r="D86" t="s">
+        <v>237</v>
+      </c>
+      <c r="E86" t="s">
+        <v>227</v>
+      </c>
+      <c r="F86" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="87" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C87" t="s">
+        <v>148</v>
+      </c>
+      <c r="D87" t="s">
+        <v>92</v>
+      </c>
+      <c r="E87" t="s">
+        <v>227</v>
+      </c>
+      <c r="F87" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="88" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C88" t="s">
+        <v>148</v>
+      </c>
+      <c r="D88" t="s">
+        <v>80</v>
+      </c>
+      <c r="E88" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="89" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C89" t="s">
+        <v>148</v>
+      </c>
+      <c r="D89" t="s">
+        <v>82</v>
+      </c>
+      <c r="E89" t="s">
+        <v>230</v>
+      </c>
+      <c r="F89" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="90" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C90" t="s">
+        <v>148</v>
+      </c>
+      <c r="D90" t="s">
+        <v>68</v>
+      </c>
+      <c r="F90" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="91" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C91" t="s">
+        <v>148</v>
+      </c>
+      <c r="D91" t="s">
+        <v>84</v>
+      </c>
+      <c r="E91" t="s">
+        <v>230</v>
+      </c>
+      <c r="F91" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="92" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C92" t="s">
+        <v>148</v>
+      </c>
+      <c r="D92" t="s">
+        <v>92</v>
+      </c>
+      <c r="E92" t="s">
+        <v>230</v>
+      </c>
+      <c r="F92" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="93" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C93" t="s">
+        <v>148</v>
+      </c>
+      <c r="D93" t="s">
+        <v>178</v>
+      </c>
+      <c r="F93" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="94" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C94" t="s">
+        <v>148</v>
+      </c>
+      <c r="D94" t="s">
         <v>180</v>
       </c>
-      <c r="F84" t="s">
+      <c r="F94" t="s">
         <v>181</v>
       </c>
     </row>
@@ -4218,8 +4354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3555E2ED-EB14-6D43-B054-42CEC3458CC1}">
   <dimension ref="A1:E71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D71" sqref="D71"/>
+    <sheetView topLeftCell="A45" workbookViewId="0">
+      <selection sqref="A1:E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5027,8 +5163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5824B443-C64F-5248-8FD1-CED7D8535BBE}">
   <dimension ref="A1:E67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Update crosswalk to check string consistency
</commit_message>
<xml_diff>
--- a/UX-Guide-Metadata/draft/localizations/crosscheck strings epub-onix-canonical_json.xlsx
+++ b/UX-Guide-Metadata/draft/localizations/crosscheck strings epub-onix-canonical_json.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/greg/Git/publ-a11y/UX-Guide-Metadata/draft/localizations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87549964-4F65-7C49-9C09-2251E1DBE2D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE3E19AA-3E30-CC4D-A4A2-F966DEA10686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17140" xr2:uid="{2FB70C81-061D-D945-B60D-ABB2568C93DD}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="865" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="228">
   <si>
     <t>id</t>
   </si>
@@ -585,90 +585,12 @@
     <t>Additional accessibility information</t>
   </si>
   <si>
-    <t>Ability to modify the appearance is not known.</t>
-  </si>
-  <si>
-    <t>Appearance can be modified.</t>
-  </si>
-  <si>
-    <t>Appearance cannot be modified.</t>
-  </si>
-  <si>
-    <t>All content is available in generated read aloud speech and electronic braille.</t>
-  </si>
-  <si>
-    <t>Readable in read aloud and braille.</t>
-  </si>
-  <si>
-    <t>May not be fully readable in read aloud and braille.</t>
-  </si>
-  <si>
-    <t>Not fully readable in read aloud and braille.</t>
-  </si>
-  <si>
-    <t>This publication meets accepted accessibility standards.</t>
-  </si>
-  <si>
     <t>Detailed Conformance Information:</t>
   </si>
   <si>
     <t>Web Accessibility Content Guidelines (WCAG) 2.1</t>
   </si>
   <si>
-    <t>Level AA.</t>
-  </si>
-  <si>
-    <t>This publication meets minimum accessibility standards.</t>
-  </si>
-  <si>
-    <t>Level A.</t>
-  </si>
-  <si>
-    <t>Audiobook with no text alternative.</t>
-  </si>
-  <si>
-    <t>Contents available as complementary audio and text.</t>
-  </si>
-  <si>
-    <t>All the content is available as pre-recorded audio synchronized with text.</t>
-  </si>
-  <si>
-    <t>Audio only.</t>
-  </si>
-  <si>
-    <t>Complementary audio and text.</t>
-  </si>
-  <si>
-    <t>Synchronized audio and text.</t>
-  </si>
-  <si>
-    <t>Contains a table of contents that provides direct access to all chapters of the text via links.</t>
-  </si>
-  <si>
-    <t>Index provides links to item references.</t>
-  </si>
-  <si>
-    <t>page list.</t>
-  </si>
-  <si>
-    <t>Charts and diagrams are present and described by extended descriptions.</t>
-  </si>
-  <si>
-    <t>Contains math formulas in accessible format.</t>
-  </si>
-  <si>
-    <t>formulas, charts, and diagrams without any information about the accessibility of this content.</t>
-  </si>
-  <si>
-    <t>Charts and diagrams have extended descriptions.</t>
-  </si>
-  <si>
-    <t>Accessible math content.</t>
-  </si>
-  <si>
-    <t>The publication contains no hazards.</t>
-  </si>
-  <si>
     <t>The publication contains</t>
   </si>
   <si>
@@ -678,9 +600,6 @@
     <t>visual stimuli or simulated movements,</t>
   </si>
   <si>
-    <t>which can cause discomfort, distraction, photosensitive seizures, or motion sickness.</t>
-  </si>
-  <si>
     <t>Flashing</t>
   </si>
   <si>
@@ -693,48 +612,12 @@
     <t>descriptive</t>
   </si>
   <si>
-    <t>Appearance of the text and page layout can be modified according to the capabilities of the reading system (font family and font size, spaces between paragraphs, sentences, words, and letters, as well as color of background and text).</t>
-  </si>
-  <si>
-    <t>Text and page layout cannot be modified. The reading experience is close to a print version. Reading systems can still provide zooming options.</t>
-  </si>
-  <si>
     <t>compact</t>
   </si>
   <si>
-    <t>Portions of the content may not be available in generated read aloud speech and electronic braille.</t>
-  </si>
-  <si>
-    <t>Not all of the content will be available in generated read aloud speech and electronic braille.</t>
-  </si>
-  <si>
-    <t>For more information, refer to the certifier's report.</t>
-  </si>
-  <si>
-    <t>A page list enables users to navigate directly to pages from the identified print source version.</t>
-  </si>
-  <si>
     <t>hasards-explanatory</t>
   </si>
   <si>
-    <t>This publication exceeds accepted accessibility standards.</t>
-  </si>
-  <si>
-    <t>The publication contains a conformance statement that it meets the EPUB Accessibility and WCAG 2 Level AAA standard.</t>
-  </si>
-  <si>
-    <t>The publication contains a conformance statement that it meets the EPUB Accessibility and WCAG 2 Level AA standard.</t>
-  </si>
-  <si>
-    <t>The publication contains a conformance statement that it meets the EPUB Accessibility and WCAG 2 Level A standard.</t>
-  </si>
-  <si>
-    <t>The publication does not include a conformance statement.</t>
-  </si>
-  <si>
-    <t>The conformance metadata is missing and conformity to a standard of this publication is unknown.</t>
-  </si>
-  <si>
     <t>Web Content Accessibility Guidelines (WCAG) 2.2</t>
   </si>
   <si>
@@ -744,24 +627,12 @@
     <t>No information about navigation is available.</t>
   </si>
   <si>
-    <t>Contains book elements such as headings, tables, etc for structured navigation.</t>
-  </si>
-  <si>
     <t>headings</t>
   </si>
   <si>
     <t>The accessibility of formulas, charts, and diagrams is not available.</t>
   </si>
   <si>
-    <t>Chemistry is in an accessible format.</t>
-  </si>
-  <si>
-    <t>Accessible chemistry content.</t>
-  </si>
-  <si>
-    <t>Accessibility of formulas, charts, and diagrams unknown.</t>
-  </si>
-  <si>
     <t>No information about possible hazards is available.</t>
   </si>
   <si>
@@ -799,6 +670,84 @@
   </si>
   <si>
     <t>ONIX string equals to principles?</t>
+  </si>
+  <si>
+    <t>Appearance of the text and page layout can be modified according to the capabilities of the reading system (font family and font size, spaces between paragraphs, sentences, words, and letters, as well as color of background and text)</t>
+  </si>
+  <si>
+    <t>Text and page layout cannot be modified as the reading experience is close to a print version, but reading systems can still provide zooming options</t>
+  </si>
+  <si>
+    <t>Ability to modify the appearance is not known</t>
+  </si>
+  <si>
+    <t>All content is available in generated read aloud speech and electronic braille</t>
+  </si>
+  <si>
+    <t>Portions of the content may not be available in generated read aloud speech and electronic braille</t>
+  </si>
+  <si>
+    <t>Not all of the content will be available in generated read aloud speech and electronic braille</t>
+  </si>
+  <si>
+    <t>The publication contains a conformance statement that it meets the EPUB Accessibility and WCAG 2 Level AAA standard</t>
+  </si>
+  <si>
+    <t>The publication contains a conformance statement that it meets the EPUB Accessibility and WCAG 2 Level AA standard</t>
+  </si>
+  <si>
+    <t>The publication contains a conformance statement that it meets the EPUB Accessibility and WCAG 2 Level A standard</t>
+  </si>
+  <si>
+    <t>The conformance metadata is missing and conformity to a standard of this publication is unknown</t>
+  </si>
+  <si>
+    <t>For more information, refer to the certifier's report</t>
+  </si>
+  <si>
+    <t>Audiobook with no text alternative</t>
+  </si>
+  <si>
+    <t>Contents available as complementary audio and text</t>
+  </si>
+  <si>
+    <t>All the content is available as pre-recorded audio synchronized with text</t>
+  </si>
+  <si>
+    <t>Contains a table of contents that provides direct access to all chapters of the text via links</t>
+  </si>
+  <si>
+    <t>Contains book elements such as headings, tables, etc for structured navigation</t>
+  </si>
+  <si>
+    <t>Index provides links to item references</t>
+  </si>
+  <si>
+    <t>A page list enables users to navigate directly to pages from the identified print source version</t>
+  </si>
+  <si>
+    <t>The accessibility of formulas, charts, and diagrams is not available</t>
+  </si>
+  <si>
+    <t>Charts and diagrams are present and described by extended descriptions</t>
+  </si>
+  <si>
+    <t>Contains math formulas in accessible format</t>
+  </si>
+  <si>
+    <t>Chemistry is in an accessible format</t>
+  </si>
+  <si>
+    <t>formulas, charts, and diagrams without any information about the accessibility of this content</t>
+  </si>
+  <si>
+    <t>The publication contains no hazards</t>
+  </si>
+  <si>
+    <t>which can cause discomfort, distraction, photosensitive seizures, or motion sickness</t>
+  </si>
+  <si>
+    <t>The presence of hazards is unknown</t>
   </si>
 </sst>
 </file>
@@ -878,37 +827,7 @@
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -946,46 +865,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1325,7 +1204,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomRight" activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1341,24 +1220,24 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>242</v>
+        <v>199</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>240</v>
+        <v>197</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>243</v>
+        <v>200</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>241</v>
+        <v>198</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>244</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="str" cm="1">
-        <f t="array" ref="A2:A89">_xlfn.UNIQUE(_xlfn.VSTACK('principles-string'!$E$2:$E$103,'epub-metadata-strings'!$D$2:$D$80,'onix-metadata-strings'!$D$2:$D$76))</f>
+        <f t="array" ref="A2:A89">_xlfn.UNIQUE(_xlfn.VSTACK('principles-string'!$E$2:$E$104,'epub-metadata-strings'!$D$2:$D$80,'onix-metadata-strings'!$D$2:$D$76))</f>
         <v>visual-adjustments-title</v>
       </c>
       <c r="B2" s="6" t="str">
@@ -1388,7 +1267,7 @@
       </c>
       <c r="B3" s="6" t="str">
         <f>IFERROR(VLOOKUP($A3&amp;"-compact",'principles-string'!$A$2:$G$1000,7,FALSE),"")</f>
-        <v>Appearance can be modified.</v>
+        <v>Appearance can be modified</v>
       </c>
       <c r="C3" s="6" t="str">
         <f>IFERROR(VLOOKUP($A3,'epub-metadata-strings'!$D$2:$E$1000,2,FALSE),"")</f>
@@ -1404,7 +1283,7 @@
       </c>
       <c r="F3" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -1413,7 +1292,7 @@
       </c>
       <c r="B4" s="6" t="str">
         <f>IFERROR(VLOOKUP($A4&amp;"-compact",'principles-string'!$A$2:$G$1000,7,FALSE),"")</f>
-        <v>Appearance cannot be modified.</v>
+        <v>Appearance cannot be modified</v>
       </c>
       <c r="C4" s="6" t="str">
         <f>IFERROR(VLOOKUP($A4,'epub-metadata-strings'!$D$2:$E$1000,2,FALSE),"")</f>
@@ -1421,7 +1300,7 @@
       </c>
       <c r="D4" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="6" t="str">
         <f>VLOOKUP($A4,'onix-metadata-strings'!$D$2:$E$1000,2,FALSE)</f>
@@ -1429,7 +1308,7 @@
       </c>
       <c r="F4" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1438,7 +1317,7 @@
       </c>
       <c r="B5" s="6" t="str">
         <f>IFERROR(VLOOKUP($A5&amp;"-compact",'principles-string'!$A$2:$G$1000,7,FALSE),"")</f>
-        <v>Ability to modify the appearance is not known.</v>
+        <v>Ability to modify the appearance is not known</v>
       </c>
       <c r="C5" s="6" t="str">
         <f>IFERROR(VLOOKUP($A5,'epub-metadata-strings'!$D$2:$E$1000,2,FALSE),"")</f>
@@ -1488,7 +1367,7 @@
       </c>
       <c r="B7" s="6" t="str">
         <f>IFERROR(VLOOKUP($A7&amp;"-compact",'principles-string'!$A$2:$G$1000,7,FALSE),"")</f>
-        <v>Readable in read aloud and braille.</v>
+        <v>Readable in read aloud and braille</v>
       </c>
       <c r="C7" s="6" t="str">
         <f>IFERROR(VLOOKUP($A7,'epub-metadata-strings'!$D$2:$E$1000,2,FALSE),"")</f>
@@ -1496,7 +1375,7 @@
       </c>
       <c r="D7" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="6" t="str">
         <f>VLOOKUP($A7,'onix-metadata-strings'!$D$2:$E$1000,2,FALSE)</f>
@@ -1504,7 +1383,7 @@
       </c>
       <c r="F7" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1513,7 +1392,7 @@
       </c>
       <c r="B8" s="6" t="str">
         <f>IFERROR(VLOOKUP($A8&amp;"-compact",'principles-string'!$A$2:$G$1000,7,FALSE),"")</f>
-        <v>May not be fully readable in read aloud and braille.</v>
+        <v>May not be fully readable in read aloud and braille</v>
       </c>
       <c r="C8" s="6" t="str">
         <f>IFERROR(VLOOKUP($A8,'epub-metadata-strings'!$D$2:$E$1000,2,FALSE),"")</f>
@@ -1521,7 +1400,7 @@
       </c>
       <c r="D8" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="6" t="str">
         <f>VLOOKUP($A8,'onix-metadata-strings'!$D$2:$E$1000,2,FALSE)</f>
@@ -1529,7 +1408,7 @@
       </c>
       <c r="F8" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1538,7 +1417,7 @@
       </c>
       <c r="B9" s="6" t="str">
         <f>IFERROR(VLOOKUP($A9&amp;"-compact",'principles-string'!$A$2:$G$1000,7,FALSE),"")</f>
-        <v>Not fully readable in read aloud and braille.</v>
+        <v>Not fully readable in read aloud and braille</v>
       </c>
       <c r="C9" s="6" t="str">
         <f>IFERROR(VLOOKUP($A9,'epub-metadata-strings'!$D$2:$E$1000,2,FALSE),"")</f>
@@ -1546,7 +1425,7 @@
       </c>
       <c r="D9" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="6" t="str">
         <f>VLOOKUP($A9,'onix-metadata-strings'!$D$2:$E$1000,2,FALSE)</f>
@@ -1554,7 +1433,7 @@
       </c>
       <c r="F9" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1588,7 +1467,7 @@
       </c>
       <c r="B11" s="6" t="str">
         <f>IFERROR(VLOOKUP($A11&amp;"-compact",'principles-string'!$A$2:$G$1000,7,FALSE),"")</f>
-        <v>This publication exceeds accepted accessibility standards.</v>
+        <v>This publication exceeds accepted accessibility standards</v>
       </c>
       <c r="C11" s="6" t="str">
         <f>IFERROR(VLOOKUP($A11,'epub-metadata-strings'!$D$2:$E$1000,2,FALSE),"")</f>
@@ -1596,7 +1475,7 @@
       </c>
       <c r="D11" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="6" t="str">
         <f>VLOOKUP($A11,'onix-metadata-strings'!$D$2:$E$1000,2,FALSE)</f>
@@ -1604,7 +1483,7 @@
       </c>
       <c r="F11" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1613,7 +1492,7 @@
       </c>
       <c r="B12" s="6" t="str">
         <f>IFERROR(VLOOKUP($A12&amp;"-compact",'principles-string'!$A$2:$G$1000,7,FALSE),"")</f>
-        <v>This publication meets accepted accessibility standards.</v>
+        <v>This publication meets accepted accessibility standards</v>
       </c>
       <c r="C12" s="6" t="str">
         <f>IFERROR(VLOOKUP($A12,'epub-metadata-strings'!$D$2:$E$1000,2,FALSE),"")</f>
@@ -1621,7 +1500,7 @@
       </c>
       <c r="D12" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="6" t="str">
         <f>VLOOKUP($A12,'onix-metadata-strings'!$D$2:$E$1000,2,FALSE)</f>
@@ -1629,7 +1508,7 @@
       </c>
       <c r="F12" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1638,7 +1517,7 @@
       </c>
       <c r="B13" s="6" t="str">
         <f>IFERROR(VLOOKUP($A13&amp;"-compact",'principles-string'!$A$2:$G$1000,7,FALSE),"")</f>
-        <v>This publication meets minimum accessibility standards.</v>
+        <v>This publication meets minimum accessibility standards</v>
       </c>
       <c r="C13" s="6" t="str">
         <f>IFERROR(VLOOKUP($A13,'epub-metadata-strings'!$D$2:$E$1000,2,FALSE),"")</f>
@@ -1646,7 +1525,7 @@
       </c>
       <c r="D13" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="6" t="str">
         <f>VLOOKUP($A13,'onix-metadata-strings'!$D$2:$E$1000,2,FALSE)</f>
@@ -1654,7 +1533,7 @@
       </c>
       <c r="F13" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1663,7 +1542,7 @@
       </c>
       <c r="B14" s="6" t="str">
         <f>IFERROR(VLOOKUP($A14&amp;"-compact",'principles-string'!$A$2:$G$1000,7,FALSE),"")</f>
-        <v>The publication does not include a conformance statement.</v>
+        <v>The publication does not include a conformance statement</v>
       </c>
       <c r="C14" s="6" t="str">
         <f>IFERROR(VLOOKUP($A14,'epub-metadata-strings'!$D$2:$E$1000,2,FALSE),"")</f>
@@ -1671,7 +1550,7 @@
       </c>
       <c r="D14" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="6" t="str">
         <f>VLOOKUP($A14,'onix-metadata-strings'!$D$2:$E$1000,2,FALSE)</f>
@@ -1679,7 +1558,7 @@
       </c>
       <c r="F14" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1738,7 +1617,7 @@
       </c>
       <c r="B17" s="6" t="str">
         <f>IFERROR(VLOOKUP($A17&amp;"-compact",'principles-string'!$A$2:$G$1000,7,FALSE),"")</f>
-        <v>The certifier's credential is</v>
+        <v>with a credential of</v>
       </c>
       <c r="C17" s="6" t="str">
         <f>IFERROR(VLOOKUP($A17,'epub-metadata-strings'!$D$2:$E$1000,2,FALSE),"")</f>
@@ -1746,7 +1625,7 @@
       </c>
       <c r="D17" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="6" t="str">
         <f>VLOOKUP($A17,'onix-metadata-strings'!$D$2:$E$1000,2,FALSE)</f>
@@ -1754,7 +1633,7 @@
       </c>
       <c r="F17" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -1863,7 +1742,7 @@
       </c>
       <c r="B22" s="6" t="str">
         <f>IFERROR(VLOOKUP($A22&amp;"-compact",'principles-string'!$A$2:$G$1000,7,FALSE),"")</f>
-        <v>Level AA.</v>
+        <v>Level AA</v>
       </c>
       <c r="C22" s="6" t="str">
         <f>IFERROR(VLOOKUP($A22,'epub-metadata-strings'!$D$2:$E$1000,2,FALSE),"")</f>
@@ -1871,7 +1750,7 @@
       </c>
       <c r="D22" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="6" t="str">
         <f>VLOOKUP($A22,'onix-metadata-strings'!$D$2:$E$1000,2,FALSE)</f>
@@ -1879,7 +1758,7 @@
       </c>
       <c r="F22" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1913,7 +1792,7 @@
       </c>
       <c r="B24" s="6" t="str">
         <f>IFERROR(VLOOKUP($A24&amp;"-compact",'principles-string'!$A$2:$G$1000,7,FALSE),"")</f>
-        <v>For more information, refer to the certifier's report.</v>
+        <v>For more information, refer to the certifier's report</v>
       </c>
       <c r="C24" s="6" t="str">
         <f>IFERROR(VLOOKUP($A24,'epub-metadata-strings'!$D$2:$E$1000,2,FALSE),"")</f>
@@ -1988,7 +1867,7 @@
       </c>
       <c r="B27" s="6" t="str">
         <f>IFERROR(VLOOKUP($A27&amp;"-compact",'principles-string'!$A$2:$G$1000,7,FALSE),"")</f>
-        <v>Level A.</v>
+        <v>Level A</v>
       </c>
       <c r="C27" s="6" t="str">
         <f>IFERROR(VLOOKUP($A27,'epub-metadata-strings'!$D$2:$E$1000,2,FALSE),"")</f>
@@ -1996,7 +1875,7 @@
       </c>
       <c r="D27" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E27" s="6" t="str">
         <f>VLOOKUP($A27,'onix-metadata-strings'!$D$2:$E$1000,2,FALSE)</f>
@@ -2004,7 +1883,7 @@
       </c>
       <c r="F27" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -2063,7 +1942,7 @@
       </c>
       <c r="B30" s="6" t="str">
         <f>IFERROR(VLOOKUP($A30&amp;"-compact",'principles-string'!$A$2:$G$1000,7,FALSE),"")</f>
-        <v>The certifier's credential is</v>
+        <v>with a credential of</v>
       </c>
       <c r="C30" s="6" t="str">
         <f>IFERROR(VLOOKUP($A30,'epub-metadata-strings'!$D$2:$E$1000,2,FALSE),"")</f>
@@ -2071,7 +1950,7 @@
       </c>
       <c r="D30" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30" s="6" t="str">
         <f>VLOOKUP($A30,'onix-metadata-strings'!$D$2:$E$1000,2,FALSE)</f>
@@ -2079,7 +1958,7 @@
       </c>
       <c r="F30" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -2138,7 +2017,7 @@
       </c>
       <c r="B33" s="6" t="str">
         <f>IFERROR(VLOOKUP($A33&amp;"-compact",'principles-string'!$A$2:$G$1000,7,FALSE),"")</f>
-        <v>Audio only.</v>
+        <v>Audio only</v>
       </c>
       <c r="C33" s="6" t="str">
         <f>IFERROR(VLOOKUP($A33,'epub-metadata-strings'!$D$2:$E$1000,2,FALSE),"")</f>
@@ -2146,7 +2025,7 @@
       </c>
       <c r="D33" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E33" s="6" t="str">
         <f>VLOOKUP($A33,'onix-metadata-strings'!$D$2:$E$1000,2,FALSE)</f>
@@ -2154,7 +2033,7 @@
       </c>
       <c r="F33" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -2163,7 +2042,7 @@
       </c>
       <c r="B34" s="6" t="str">
         <f>IFERROR(VLOOKUP($A34&amp;"-compact",'principles-string'!$A$2:$G$1000,7,FALSE),"")</f>
-        <v>Complementary audio and text.</v>
+        <v>Complementary audio and text</v>
       </c>
       <c r="C34" s="6" t="str">
         <f>IFERROR(VLOOKUP($A34,'epub-metadata-strings'!$D$2:$E$1000,2,FALSE),"")</f>
@@ -2171,7 +2050,7 @@
       </c>
       <c r="D34" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E34" s="6" t="str">
         <f>VLOOKUP($A34,'onix-metadata-strings'!$D$2:$E$1000,2,FALSE)</f>
@@ -2179,7 +2058,7 @@
       </c>
       <c r="F34" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -2188,7 +2067,7 @@
       </c>
       <c r="B35" s="6" t="str">
         <f>IFERROR(VLOOKUP($A35&amp;"-compact",'principles-string'!$A$2:$G$1000,7,FALSE),"")</f>
-        <v>Synchronized audio and text.</v>
+        <v>Synchronized audio and text</v>
       </c>
       <c r="C35" s="6" t="str">
         <f>IFERROR(VLOOKUP($A35,'epub-metadata-strings'!$D$2:$E$1000,2,FALSE),"")</f>
@@ -2196,7 +2075,7 @@
       </c>
       <c r="D35" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E35" s="6" t="str">
         <f>VLOOKUP($A35,'onix-metadata-strings'!$D$2:$E$1000,2,FALSE)</f>
@@ -2204,7 +2083,7 @@
       </c>
       <c r="F35" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -2338,7 +2217,7 @@
       </c>
       <c r="B41" s="6" t="str">
         <f>IFERROR(VLOOKUP($A41&amp;"-compact",'principles-string'!$A$2:$G$1000,7,FALSE),"")</f>
-        <v>page list.</v>
+        <v>supports page navigation</v>
       </c>
       <c r="C41" s="6" t="str">
         <f>IFERROR(VLOOKUP($A41,'epub-metadata-strings'!$D$2:$E$1000,2,FALSE),"")</f>
@@ -2346,7 +2225,7 @@
       </c>
       <c r="D41" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E41" s="6" t="str">
         <f>VLOOKUP($A41,'onix-metadata-strings'!$D$2:$E$1000,2,FALSE)</f>
@@ -2354,7 +2233,7 @@
       </c>
       <c r="F41" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -2438,7 +2317,7 @@
       </c>
       <c r="B45" s="6" t="str">
         <f>IFERROR(VLOOKUP($A45&amp;"-compact",'principles-string'!$A$2:$G$1000,7,FALSE),"")</f>
-        <v>Accessibility of formulas, charts, and diagrams unknown.</v>
+        <v>The accessibility of formulas, charts, and diagrams is not available</v>
       </c>
       <c r="C45" s="6" t="str">
         <f>IFERROR(VLOOKUP($A45,'epub-metadata-strings'!$D$2:$E$1000,2,FALSE),"")</f>
@@ -2463,7 +2342,7 @@
       </c>
       <c r="B46" s="6" t="str">
         <f>IFERROR(VLOOKUP($A46&amp;"-compact",'principles-string'!$A$2:$G$1000,7,FALSE),"")</f>
-        <v>Charts and diagrams have extended descriptions.</v>
+        <v>Charts and diagrams have extended descriptions</v>
       </c>
       <c r="C46" s="6" t="str">
         <f>IFERROR(VLOOKUP($A46,'epub-metadata-strings'!$D$2:$E$1000,2,FALSE),"")</f>
@@ -2471,7 +2350,7 @@
       </c>
       <c r="D46" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E46" s="6" t="str">
         <f>VLOOKUP($A46,'onix-metadata-strings'!$D$2:$E$1000,2,FALSE)</f>
@@ -2479,7 +2358,7 @@
       </c>
       <c r="F46" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
@@ -2488,7 +2367,7 @@
       </c>
       <c r="B47" s="6" t="str">
         <f>IFERROR(VLOOKUP($A47&amp;"-compact",'principles-string'!$A$2:$G$1000,7,FALSE),"")</f>
-        <v>Accessible math content.</v>
+        <v>Accessible math content</v>
       </c>
       <c r="C47" s="6" t="str">
         <f>IFERROR(VLOOKUP($A47,'epub-metadata-strings'!$D$2:$E$1000,2,FALSE),"")</f>
@@ -2496,7 +2375,7 @@
       </c>
       <c r="D47" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E47" s="6" t="str">
         <f>VLOOKUP($A47,'onix-metadata-strings'!$D$2:$E$1000,2,FALSE)</f>
@@ -2504,7 +2383,7 @@
       </c>
       <c r="F47" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
@@ -2513,7 +2392,7 @@
       </c>
       <c r="B48" s="6" t="str">
         <f>IFERROR(VLOOKUP($A48&amp;"-compact",'principles-string'!$A$2:$G$1000,7,FALSE),"")</f>
-        <v>Accessible chemistry content.</v>
+        <v>Accessible chemistry content</v>
       </c>
       <c r="C48" s="6" t="str">
         <f>IFERROR(VLOOKUP($A48,'epub-metadata-strings'!$D$2:$E$1000,2,FALSE),"")</f>
@@ -2521,7 +2400,7 @@
       </c>
       <c r="D48" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E48" s="6" t="str">
         <f>VLOOKUP($A48,'onix-metadata-strings'!$D$2:$E$1000,2,FALSE)</f>
@@ -2529,7 +2408,7 @@
       </c>
       <c r="F48" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
@@ -2713,7 +2592,7 @@
       </c>
       <c r="B56" s="6" t="str">
         <f>IFERROR(VLOOKUP($A56&amp;"-compact",'principles-string'!$A$2:$G$1000,7,FALSE),"")</f>
-        <v>The presence of hazards is unknown.</v>
+        <v>The presence of hazards is unknown</v>
       </c>
       <c r="C56" s="6" t="str">
         <f>IFERROR(VLOOKUP($A56,'epub-metadata-strings'!$D$2:$E$1000,2,FALSE),"")</f>
@@ -2721,7 +2600,7 @@
       </c>
       <c r="D56" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E56" s="6" t="str">
         <f>VLOOKUP($A56,'onix-metadata-strings'!$D$2:$E$1000,2,FALSE)</f>
@@ -2729,7 +2608,7 @@
       </c>
       <c r="F56" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
@@ -4048,18 +3927,18 @@
   </sheetData>
   <autoFilter ref="A1:E90" xr:uid="{3A9EDDE9-AF31-2D43-AC52-4CD1D03679BB}"/>
   <conditionalFormatting sqref="D2:D89">
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>TRUE</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
-      <formula>FALSE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F89">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4069,10 +3948,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DAAE526-051A-2147-9F70-F78890C8D07D}">
-  <dimension ref="A1:G103"/>
+  <dimension ref="A1:G104"/>
   <sheetViews>
-    <sheetView topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4084,7 +3963,7 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>239</v>
+        <v>196</v>
       </c>
       <c r="B1" t="s">
         <v>135</v>
@@ -4099,7 +3978,7 @@
         <v>138</v>
       </c>
       <c r="F1" t="s">
-        <v>206</v>
+        <v>179</v>
       </c>
       <c r="G1" t="s">
         <v>139</v>
@@ -4117,7 +3996,7 @@
         <v>141</v>
       </c>
       <c r="E2" t="s">
-        <v>207</v>
+        <v>180</v>
       </c>
       <c r="G2" t="s">
         <v>156</v>
@@ -4135,10 +4014,10 @@
         <v>114</v>
       </c>
       <c r="F3" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="G3" t="s">
-        <v>209</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -4153,10 +4032,10 @@
         <v>115</v>
       </c>
       <c r="F4" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="G4" t="s">
-        <v>210</v>
+        <v>203</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -4171,10 +4050,10 @@
         <v>116</v>
       </c>
       <c r="F5" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="G5" t="s">
-        <v>173</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -4189,10 +4068,10 @@
         <v>114</v>
       </c>
       <c r="F6" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="G6" t="s">
-        <v>174</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -4207,10 +4086,10 @@
         <v>115</v>
       </c>
       <c r="F7" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="G7" t="s">
-        <v>175</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -4225,10 +4104,10 @@
         <v>116</v>
       </c>
       <c r="F8" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="G8" t="s">
-        <v>173</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -4258,10 +4137,10 @@
         <v>3</v>
       </c>
       <c r="F10" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="G10" t="s">
-        <v>176</v>
+        <v>205</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -4276,10 +4155,10 @@
         <v>7</v>
       </c>
       <c r="F11" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="G11" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -4294,10 +4173,10 @@
         <v>5</v>
       </c>
       <c r="F12" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="G12" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -4312,10 +4191,10 @@
         <v>3</v>
       </c>
       <c r="F13" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="G13" t="s">
-        <v>177</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -4330,10 +4209,10 @@
         <v>7</v>
       </c>
       <c r="F14" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="G14" t="s">
-        <v>178</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -4348,10 +4227,10 @@
         <v>5</v>
       </c>
       <c r="F15" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="G15" t="s">
-        <v>179</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -4381,10 +4260,10 @@
         <v>9</v>
       </c>
       <c r="F17" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="G17" t="s">
-        <v>217</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -4399,10 +4278,10 @@
         <v>9</v>
       </c>
       <c r="F18" t="s">
+        <v>181</v>
+      </c>
+      <c r="G18" t="s">
         <v>208</v>
-      </c>
-      <c r="G18" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -4417,10 +4296,10 @@
         <v>11</v>
       </c>
       <c r="F19" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="G19" t="s">
-        <v>180</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -4435,10 +4314,10 @@
         <v>11</v>
       </c>
       <c r="F20" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="G20" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -4453,10 +4332,10 @@
         <v>13</v>
       </c>
       <c r="F21" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="G21" t="s">
-        <v>184</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -4471,10 +4350,10 @@
         <v>13</v>
       </c>
       <c r="F22" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="G22" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -4489,10 +4368,10 @@
         <v>16</v>
       </c>
       <c r="F23" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="G23" t="s">
-        <v>221</v>
+        <v>17</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -4507,10 +4386,10 @@
         <v>16</v>
       </c>
       <c r="F24" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="G24" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -4525,10 +4404,10 @@
         <v>11</v>
       </c>
       <c r="F25" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="G25" t="s">
-        <v>180</v>
+        <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -4543,7 +4422,7 @@
         <v>42</v>
       </c>
       <c r="F26" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="G26" t="s">
         <v>43</v>
@@ -4561,7 +4440,7 @@
         <v>45</v>
       </c>
       <c r="F27" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="G27" t="s">
         <v>46</v>
@@ -4579,10 +4458,10 @@
         <v>47</v>
       </c>
       <c r="F28" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="G28" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -4597,7 +4476,7 @@
         <v>22</v>
       </c>
       <c r="G29" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -4642,10 +4521,10 @@
         <v>32</v>
       </c>
       <c r="F32" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="G32" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -4660,7 +4539,7 @@
         <v>38</v>
       </c>
       <c r="G33" t="s">
-        <v>183</v>
+        <v>39</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -4675,7 +4554,7 @@
         <v>42</v>
       </c>
       <c r="F34" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="G34" t="s">
         <v>43</v>
@@ -4708,7 +4587,7 @@
         <v>45</v>
       </c>
       <c r="F36" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="G36" t="s">
         <v>46</v>
@@ -4741,7 +4620,7 @@
         <v>49</v>
       </c>
       <c r="G38" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -4756,10 +4635,10 @@
         <v>13</v>
       </c>
       <c r="F39" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="G39" t="s">
-        <v>184</v>
+        <v>14</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -4774,7 +4653,7 @@
         <v>42</v>
       </c>
       <c r="F40" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="G40" t="s">
         <v>43</v>
@@ -4792,7 +4671,7 @@
         <v>45</v>
       </c>
       <c r="F41" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="G41" t="s">
         <v>46</v>
@@ -4810,10 +4689,10 @@
         <v>47</v>
       </c>
       <c r="F42" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="G42" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -4828,7 +4707,7 @@
         <v>22</v>
       </c>
       <c r="G43" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -4873,10 +4752,10 @@
         <v>34</v>
       </c>
       <c r="F46" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="G46" t="s">
-        <v>223</v>
+        <v>184</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -4891,7 +4770,7 @@
         <v>40</v>
       </c>
       <c r="G47" t="s">
-        <v>185</v>
+        <v>41</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -4906,7 +4785,7 @@
         <v>42</v>
       </c>
       <c r="F48" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="G48" t="s">
         <v>43</v>
@@ -4939,7 +4818,7 @@
         <v>45</v>
       </c>
       <c r="F50" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="G50" t="s">
         <v>46</v>
@@ -4972,7 +4851,7 @@
         <v>49</v>
       </c>
       <c r="G52" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
@@ -4984,7 +4863,7 @@
         <v>141</v>
       </c>
       <c r="E53" t="s">
-        <v>237</v>
+        <v>194</v>
       </c>
       <c r="G53" t="s">
         <v>15</v>
@@ -5017,837 +4896,855 @@
         <v>20</v>
       </c>
       <c r="G55" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>pre-recorded-audio-title-compact</v>
+        <v>conformance-no-compact</v>
       </c>
       <c r="D56" t="s">
         <v>141</v>
       </c>
       <c r="E56" t="s">
-        <v>161</v>
+        <v>16</v>
+      </c>
+      <c r="F56" t="s">
+        <v>182</v>
       </c>
       <c r="G56" t="s">
-        <v>162</v>
+        <v>17</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>pre-recorded-audio-no-metadata-descriptive</v>
+        <v>pre-recorded-audio-title-compact</v>
       </c>
       <c r="D57" t="s">
         <v>141</v>
       </c>
       <c r="E57" t="s">
-        <v>57</v>
-      </c>
-      <c r="F57" t="s">
-        <v>208</v>
+        <v>161</v>
       </c>
       <c r="G57" t="s">
-        <v>224</v>
+        <v>162</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>pre-recorded-audio-only-descriptive</v>
+        <v>pre-recorded-audio-no-metadata-descriptive</v>
       </c>
       <c r="D58" t="s">
         <v>141</v>
       </c>
       <c r="E58" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="F58" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="G58" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>pre-recorded-audio-complementary-descriptive</v>
+        <v>pre-recorded-audio-only-descriptive</v>
       </c>
       <c r="D59" t="s">
         <v>141</v>
       </c>
       <c r="E59" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F59" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="G59" t="s">
-        <v>187</v>
+        <v>213</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>pre-recorded-audio-synchronized-descriptive</v>
+        <v>pre-recorded-audio-complementary-descriptive</v>
       </c>
       <c r="D60" t="s">
         <v>141</v>
       </c>
       <c r="E60" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F60" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="G60" t="s">
-        <v>188</v>
+        <v>214</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>pre-recorded-audio-only-compact</v>
+        <v>pre-recorded-audio-synchronized-descriptive</v>
       </c>
       <c r="D61" t="s">
         <v>141</v>
       </c>
       <c r="E61" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F61" t="s">
-        <v>211</v>
+        <v>181</v>
       </c>
       <c r="G61" t="s">
-        <v>189</v>
+        <v>215</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>pre-recorded-audio-complementary-compact</v>
+        <v>pre-recorded-audio-only-compact</v>
       </c>
       <c r="D62" t="s">
         <v>141</v>
       </c>
       <c r="E62" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="F62" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="G62" t="s">
-        <v>190</v>
+        <v>52</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>pre-recorded-audio-synchronized-compact</v>
+        <v>pre-recorded-audio-complementary-compact</v>
       </c>
       <c r="D63" t="s">
         <v>141</v>
       </c>
       <c r="E63" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="F63" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="G63" t="s">
-        <v>191</v>
+        <v>56</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>navigation-title-compact</v>
+        <v>pre-recorded-audio-synchronized-compact</v>
       </c>
       <c r="D64" t="s">
         <v>141</v>
       </c>
       <c r="E64" t="s">
-        <v>163</v>
+        <v>53</v>
+      </c>
+      <c r="F64" t="s">
+        <v>182</v>
       </c>
       <c r="G64" t="s">
-        <v>164</v>
+        <v>54</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>navigation-no-metadata-descriptive</v>
+        <v>navigation-title-compact</v>
       </c>
       <c r="D65" t="s">
         <v>141</v>
       </c>
       <c r="E65" t="s">
-        <v>69</v>
-      </c>
-      <c r="F65" t="s">
-        <v>208</v>
+        <v>163</v>
       </c>
       <c r="G65" t="s">
-        <v>225</v>
+        <v>164</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="str">
         <f t="shared" si="0"/>
-        <v>navigation-toc-descriptive</v>
+        <v>navigation-no-metadata-descriptive</v>
       </c>
       <c r="D66" t="s">
         <v>141</v>
       </c>
       <c r="E66" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="F66" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="G66" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="str">
-        <f t="shared" ref="A67:A103" si="1">E67&amp;"-"&amp;IF(ISBLANK(F67),"compact",F67)</f>
-        <v>navigation-structural-descriptive</v>
+        <f t="shared" ref="A67:A104" si="1">E67&amp;"-"&amp;IF(ISBLANK(F67),"compact",F67)</f>
+        <v>navigation-toc-descriptive</v>
       </c>
       <c r="D67" t="s">
         <v>141</v>
       </c>
       <c r="E67" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F67" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="G67" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>navigation-index-descriptive</v>
+        <v>navigation-structural-descriptive</v>
       </c>
       <c r="D68" t="s">
         <v>141</v>
       </c>
       <c r="E68" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F68" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="G68" t="s">
-        <v>193</v>
+        <v>217</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>navigation-page-navigation-descriptive</v>
+        <v>navigation-index-descriptive</v>
       </c>
       <c r="D69" t="s">
         <v>141</v>
       </c>
       <c r="E69" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F69" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="G69" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>navigation-intro-compact</v>
+        <v>navigation-page-navigation-descriptive</v>
       </c>
       <c r="D70" t="s">
         <v>141</v>
       </c>
       <c r="E70" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="F70" t="s">
-        <v>211</v>
+        <v>181</v>
       </c>
       <c r="G70" t="s">
-        <v>68</v>
+        <v>219</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>navigation-toc-compact</v>
+        <v>navigation-intro-compact</v>
       </c>
       <c r="D71" t="s">
         <v>141</v>
       </c>
       <c r="E71" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="F71" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="G71" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>navigation-structural-compact</v>
+        <v>navigation-toc-compact</v>
       </c>
       <c r="D72" t="s">
         <v>141</v>
       </c>
       <c r="E72" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F72" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="G72" t="s">
-        <v>227</v>
+        <v>59</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>navigation-index-compact</v>
+        <v>navigation-structural-compact</v>
       </c>
       <c r="D73" t="s">
         <v>141</v>
       </c>
       <c r="E73" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="F73" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="G73" t="s">
-        <v>61</v>
+        <v>187</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>join-array-and-compact</v>
+        <v>navigation-index-compact</v>
       </c>
       <c r="D74" t="s">
         <v>141</v>
       </c>
       <c r="E74" t="s">
-        <v>66</v>
+        <v>60</v>
+      </c>
+      <c r="F74" t="s">
+        <v>182</v>
       </c>
       <c r="G74" t="s">
-        <v>117</v>
+        <v>61</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>navigation-page-navigation-compact</v>
+        <v>join-array-and-compact</v>
       </c>
       <c r="D75" t="s">
         <v>141</v>
       </c>
       <c r="E75" t="s">
-        <v>63</v>
-      </c>
-      <c r="F75" t="s">
-        <v>211</v>
+        <v>66</v>
       </c>
       <c r="G75" t="s">
-        <v>194</v>
+        <v>117</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>charts-diagrams-formulas-title-compact</v>
+        <v>navigation-page-navigation-compact</v>
       </c>
       <c r="D76" t="s">
         <v>141</v>
       </c>
       <c r="E76" t="s">
-        <v>165</v>
+        <v>63</v>
+      </c>
+      <c r="F76" t="s">
+        <v>182</v>
       </c>
       <c r="G76" t="s">
-        <v>166</v>
+        <v>132</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>charts-diagrams-formulas-unknown-descriptive</v>
+        <v>charts-diagrams-formulas-title-compact</v>
       </c>
       <c r="D77" t="s">
         <v>141</v>
       </c>
       <c r="E77" t="s">
-        <v>133</v>
-      </c>
-      <c r="F77" t="s">
-        <v>208</v>
+        <v>165</v>
       </c>
       <c r="G77" t="s">
-        <v>228</v>
+        <v>166</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>charts-diagrams-formulas-extended-descriptive</v>
+        <v>charts-diagrams-formulas-unknown-descriptive</v>
       </c>
       <c r="D78" t="s">
         <v>141</v>
       </c>
       <c r="E78" t="s">
-        <v>70</v>
+        <v>133</v>
       </c>
       <c r="F78" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="G78" t="s">
-        <v>195</v>
+        <v>220</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>charts-diagrams-formulas-accessible-math-descriptive</v>
+        <v>charts-diagrams-formulas-extended-descriptive</v>
       </c>
       <c r="D79" t="s">
         <v>141</v>
       </c>
       <c r="E79" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F79" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="G79" t="s">
-        <v>196</v>
+        <v>221</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>charts-diagrams-formulas-accessible-chemistry-descriptive</v>
+        <v>charts-diagrams-formulas-accessible-math-descriptive</v>
       </c>
       <c r="D80" t="s">
         <v>141</v>
       </c>
       <c r="E80" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F80" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="G80" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>charts-diagrams-formulas-unknown-descriptive</v>
+        <v>charts-diagrams-formulas-accessible-chemistry-descriptive</v>
       </c>
       <c r="D81" t="s">
         <v>141</v>
       </c>
       <c r="E81" t="s">
-        <v>133</v>
+        <v>72</v>
       </c>
       <c r="F81" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="G81" t="s">
-        <v>197</v>
+        <v>223</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>charts-diagrams-formulas-extended-compact</v>
+        <v>charts-diagrams-formulas-unknown-descriptive</v>
       </c>
       <c r="D82" t="s">
         <v>141</v>
       </c>
       <c r="E82" t="s">
-        <v>70</v>
+        <v>133</v>
       </c>
       <c r="F82" t="s">
-        <v>211</v>
+        <v>181</v>
       </c>
       <c r="G82" t="s">
-        <v>198</v>
+        <v>224</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>charts-diagrams-formulas-accessible-math-compact</v>
+        <v>charts-diagrams-formulas-extended-compact</v>
       </c>
       <c r="D83" t="s">
         <v>141</v>
       </c>
       <c r="E83" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F83" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="G83" t="s">
-        <v>199</v>
+        <v>71</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>charts-diagrams-formulas-accessible-chemistry-compact</v>
+        <v>charts-diagrams-formulas-accessible-math-compact</v>
       </c>
       <c r="D84" t="s">
         <v>141</v>
       </c>
       <c r="E84" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F84" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="G84" t="s">
-        <v>230</v>
+        <v>75</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>charts-diagrams-formulas-unknown-compact</v>
+        <v>charts-diagrams-formulas-accessible-chemistry-compact</v>
       </c>
       <c r="D85" t="s">
         <v>141</v>
       </c>
       <c r="E85" t="s">
-        <v>133</v>
+        <v>72</v>
       </c>
       <c r="F85" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="G85" t="s">
-        <v>231</v>
+        <v>73</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>hazards-title-compact</v>
+        <v>charts-diagrams-formulas-unknown-compact</v>
       </c>
       <c r="D86" t="s">
         <v>141</v>
       </c>
       <c r="E86" t="s">
-        <v>167</v>
+        <v>133</v>
+      </c>
+      <c r="F86" t="s">
+        <v>182</v>
       </c>
       <c r="G86" t="s">
-        <v>168</v>
+        <v>220</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>hazards-no-metadata-descriptive</v>
+        <v>hazards-title-compact</v>
       </c>
       <c r="D87" t="s">
         <v>141</v>
       </c>
       <c r="E87" t="s">
-        <v>89</v>
-      </c>
-      <c r="F87" t="s">
-        <v>208</v>
+        <v>167</v>
       </c>
       <c r="G87" t="s">
-        <v>232</v>
+        <v>168</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>hazards-none-descriptive</v>
+        <v>hazards-no-metadata-descriptive</v>
       </c>
       <c r="D88" t="s">
         <v>141</v>
       </c>
       <c r="E88" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="F88" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="G88" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>hazards-flashing-descriptive</v>
+        <v>hazards-none-descriptive</v>
       </c>
       <c r="D89" t="s">
         <v>141</v>
       </c>
       <c r="E89" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F89" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="G89" t="s">
-        <v>201</v>
+        <v>225</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>hazards-sound-descriptive</v>
+        <v>hazards-flashing-descriptive</v>
       </c>
       <c r="D90" t="s">
         <v>141</v>
       </c>
       <c r="E90" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F90" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="G90" t="s">
-        <v>202</v>
+        <v>175</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>hazards-motion-descriptive</v>
+        <v>hazards-sound-descriptive</v>
       </c>
       <c r="D91" t="s">
         <v>141</v>
       </c>
       <c r="E91" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="F91" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="G91" t="s">
-        <v>203</v>
+        <v>176</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>hasards-explanatory-descriptive</v>
+        <v>hazards-motion-descriptive</v>
       </c>
       <c r="D92" t="s">
         <v>141</v>
       </c>
       <c r="E92" t="s">
-        <v>216</v>
+        <v>80</v>
       </c>
       <c r="F92" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="G92" t="s">
-        <v>204</v>
+        <v>177</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A93" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>hazards-unknown-descriptive</v>
+        <v>hasards-explanatory-descriptive</v>
       </c>
       <c r="D93" t="s">
         <v>141</v>
       </c>
       <c r="E93" t="s">
-        <v>88</v>
+        <v>183</v>
       </c>
       <c r="F93" t="s">
-        <v>208</v>
+        <v>181</v>
       </c>
       <c r="G93" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>hazards-none-compact</v>
+        <v>hazards-unknown-descriptive</v>
       </c>
       <c r="D94" t="s">
         <v>141</v>
       </c>
       <c r="E94" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="F94" t="s">
-        <v>211</v>
+        <v>181</v>
+      </c>
+      <c r="G94" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>hazards-flashing-compact</v>
+        <v>hazards-none-compact</v>
       </c>
       <c r="D95" t="s">
         <v>141</v>
       </c>
       <c r="E95" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F95" t="s">
-        <v>211</v>
-      </c>
-      <c r="G95" t="s">
-        <v>205</v>
+        <v>182</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A96" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>join-array-and-compact</v>
+        <v>hazards-flashing-compact</v>
       </c>
       <c r="D96" t="s">
         <v>141</v>
       </c>
       <c r="E96" t="s">
-        <v>66</v>
+        <v>78</v>
+      </c>
+      <c r="F96" t="s">
+        <v>182</v>
       </c>
       <c r="G96" t="s">
-        <v>117</v>
+        <v>178</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A97" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>hazards-motion-compact</v>
+        <v>join-array-and-compact</v>
       </c>
       <c r="D97" t="s">
         <v>141</v>
       </c>
       <c r="E97" t="s">
-        <v>80</v>
-      </c>
-      <c r="F97" t="s">
-        <v>211</v>
+        <v>66</v>
       </c>
       <c r="G97" t="s">
-        <v>238</v>
+        <v>117</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A98" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>hazards-plural-compact</v>
+        <v>hazards-motion-compact</v>
       </c>
       <c r="D98" t="s">
         <v>141</v>
       </c>
       <c r="E98" t="s">
-        <v>84</v>
+        <v>80</v>
+      </c>
+      <c r="F98" t="s">
+        <v>182</v>
       </c>
       <c r="G98" t="s">
-        <v>85</v>
+        <v>195</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A99" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>hazards-unknown-compact</v>
+        <v>hazards-plural-compact</v>
       </c>
       <c r="D99" t="s">
         <v>141</v>
       </c>
       <c r="E99" t="s">
-        <v>88</v>
-      </c>
-      <c r="F99" t="s">
-        <v>211</v>
+        <v>84</v>
       </c>
       <c r="G99" t="s">
-        <v>233</v>
+        <v>85</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A100" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>accessibility-summary-title-compact</v>
+        <v>hazards-unknown-compact</v>
       </c>
       <c r="D100" t="s">
         <v>141</v>
       </c>
       <c r="E100" t="s">
-        <v>169</v>
+        <v>88</v>
+      </c>
+      <c r="F100" t="s">
+        <v>182</v>
       </c>
       <c r="G100" t="s">
-        <v>170</v>
+        <v>227</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A101" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>accessibility-summary-no-metadata-descriptive</v>
+        <v>accessibility-summary-title-compact</v>
       </c>
       <c r="D101" t="s">
         <v>141</v>
       </c>
       <c r="E101" t="s">
-        <v>90</v>
-      </c>
-      <c r="F101" t="s">
-        <v>208</v>
+        <v>169</v>
       </c>
       <c r="G101" t="s">
-        <v>234</v>
+        <v>170</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A102" s="4" t="str">
         <f t="shared" si="1"/>
-        <v>legal-considerations-title-compact</v>
+        <v>accessibility-summary-no-metadata-descriptive</v>
       </c>
       <c r="D102" t="s">
         <v>141</v>
       </c>
       <c r="E102" t="s">
-        <v>235</v>
+        <v>90</v>
+      </c>
+      <c r="F102" t="s">
+        <v>181</v>
       </c>
       <c r="G102" t="s">
-        <v>236</v>
+        <v>191</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A103" s="4" t="str">
         <f t="shared" si="1"/>
+        <v>legal-considerations-title-compact</v>
+      </c>
+      <c r="D103" t="s">
+        <v>141</v>
+      </c>
+      <c r="E103" t="s">
+        <v>192</v>
+      </c>
+      <c r="G103" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A104" s="4" t="str">
+        <f t="shared" si="1"/>
         <v>additional-accessibility-information-title-compact</v>
       </c>
-      <c r="D103" t="s">
-        <v>141</v>
-      </c>
-      <c r="E103" t="s">
+      <c r="D104" t="s">
+        <v>141</v>
+      </c>
+      <c r="E104" t="s">
         <v>171</v>
       </c>
-      <c r="G103" t="s">
+      <c r="G104" t="s">
         <v>172</v>
       </c>
     </row>
@@ -5860,8 +5757,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3555E2ED-EB14-6D43-B054-42CEC3458CC1}">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="D80" sqref="D80"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E88" sqref="E88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5906,7 +5803,7 @@
         <v>141</v>
       </c>
       <c r="D3" t="s">
-        <v>207</v>
+        <v>180</v>
       </c>
       <c r="E3" t="s">
         <v>156</v>
@@ -6038,7 +5935,7 @@
         <v>141</v>
       </c>
       <c r="D15" t="s">
-        <v>237</v>
+        <v>194</v>
       </c>
       <c r="E15" t="s">
         <v>15</v>
@@ -6294,7 +6191,7 @@
         <v>57</v>
       </c>
       <c r="E38" t="s">
-        <v>224</v>
+        <v>185</v>
       </c>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.2">
@@ -6371,7 +6268,7 @@
         <v>69</v>
       </c>
       <c r="E45" t="s">
-        <v>225</v>
+        <v>186</v>
       </c>
     </row>
     <row r="46" spans="3:5" x14ac:dyDescent="0.2">
@@ -6426,7 +6323,7 @@
         <v>133</v>
       </c>
       <c r="E50" t="s">
-        <v>228</v>
+        <v>188</v>
       </c>
     </row>
     <row r="51" spans="3:5" x14ac:dyDescent="0.2">
@@ -6514,7 +6411,7 @@
         <v>88</v>
       </c>
       <c r="E58" t="s">
-        <v>233</v>
+        <v>190</v>
       </c>
     </row>
     <row r="59" spans="3:5" x14ac:dyDescent="0.2">
@@ -6525,7 +6422,7 @@
         <v>89</v>
       </c>
       <c r="E59" t="s">
-        <v>232</v>
+        <v>189</v>
       </c>
     </row>
     <row r="60" spans="3:5" x14ac:dyDescent="0.2">
@@ -6547,7 +6444,7 @@
         <v>90</v>
       </c>
       <c r="E61" t="s">
-        <v>234</v>
+        <v>191</v>
       </c>
     </row>
     <row r="62" spans="3:5" x14ac:dyDescent="0.2">
@@ -6555,10 +6452,10 @@
         <v>141</v>
       </c>
       <c r="D62" t="s">
-        <v>235</v>
+        <v>192</v>
       </c>
       <c r="E62" t="s">
-        <v>236</v>
+        <v>193</v>
       </c>
     </row>
     <row r="63" spans="3:5" x14ac:dyDescent="0.2">
@@ -6768,8 +6665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5824B443-C64F-5248-8FD1-CED7D8535BBE}">
   <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="D76" sqref="D76"/>
+    <sheetView topLeftCell="A68" workbookViewId="0">
+      <selection activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6814,7 +6711,7 @@
         <v>141</v>
       </c>
       <c r="D3" t="s">
-        <v>207</v>
+        <v>180</v>
       </c>
       <c r="E3" t="s">
         <v>156</v>
@@ -7191,7 +7088,7 @@
         <v>57</v>
       </c>
       <c r="E37" t="s">
-        <v>224</v>
+        <v>185</v>
       </c>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.2">
@@ -7268,7 +7165,7 @@
         <v>69</v>
       </c>
       <c r="E44" t="s">
-        <v>225</v>
+        <v>186</v>
       </c>
     </row>
     <row r="45" spans="3:5" x14ac:dyDescent="0.2">
@@ -7334,7 +7231,7 @@
         <v>133</v>
       </c>
       <c r="E50" t="s">
-        <v>228</v>
+        <v>188</v>
       </c>
     </row>
     <row r="51" spans="3:5" x14ac:dyDescent="0.2">
@@ -7422,7 +7319,7 @@
         <v>88</v>
       </c>
       <c r="E58" t="s">
-        <v>233</v>
+        <v>190</v>
       </c>
     </row>
     <row r="59" spans="3:5" x14ac:dyDescent="0.2">
@@ -7433,7 +7330,7 @@
         <v>89</v>
       </c>
       <c r="E59" t="s">
-        <v>232</v>
+        <v>189</v>
       </c>
     </row>
     <row r="60" spans="3:5" x14ac:dyDescent="0.2">
@@ -7455,7 +7352,7 @@
         <v>90</v>
       </c>
       <c r="E61" t="s">
-        <v>234</v>
+        <v>191</v>
       </c>
     </row>
     <row r="62" spans="3:5" x14ac:dyDescent="0.2">
@@ -7463,10 +7360,10 @@
         <v>141</v>
       </c>
       <c r="D62" t="s">
-        <v>235</v>
+        <v>192</v>
       </c>
       <c r="E62" t="s">
-        <v>236</v>
+        <v>193</v>
       </c>
     </row>
     <row r="63" spans="3:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update crosscheck strings epub-onix-canonical_json.xlsx
</commit_message>
<xml_diff>
--- a/UX-Guide-Metadata/draft/localizations/crosscheck strings epub-onix-canonical_json.xlsx
+++ b/UX-Guide-Metadata/draft/localizations/crosscheck strings epub-onix-canonical_json.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/greg/Git/publ-a11y/UX-Guide-Metadata/draft/localizations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE3E19AA-3E30-CC4D-A4A2-F966DEA10686}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A005B1-C04F-094E-A59A-EB7BCFA0C838}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17140" xr2:uid="{2FB70C81-061D-D945-B60D-ABB2568C93DD}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="29400" windowHeight="17040" xr2:uid="{2FB70C81-061D-D945-B60D-ABB2568C93DD}"/>
   </bookViews>
   <sheets>
     <sheet name="crosscheck" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="869" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="218">
   <si>
     <t>id</t>
   </si>
@@ -216,9 +216,6 @@
     <t>conformance-certifier-report</t>
   </si>
   <si>
-    <t>For more information refer to the certifier's report.</t>
-  </si>
-  <si>
     <t>pre-recorded-audio-only</t>
   </si>
   <si>
@@ -261,9 +258,6 @@
     <t>navigation-structural</t>
   </si>
   <si>
-    <t>structural navigation</t>
-  </si>
-  <si>
     <t>join-array-and</t>
   </si>
   <si>
@@ -309,9 +303,6 @@
     <t>hazards-motion</t>
   </si>
   <si>
-    <t>motion</t>
-  </si>
-  <si>
     <t>hazards-sound</t>
   </si>
   <si>
@@ -492,9 +483,6 @@
     <t/>
   </si>
   <si>
-    <t>ppearance can be modified</t>
-  </si>
-  <si>
     <t>conformance-certification-date-prefix</t>
   </si>
   <si>
@@ -564,9 +552,6 @@
     <t>charts-diagrams-formulas-title</t>
   </si>
   <si>
-    <t>Charts, diagrams, and formulas</t>
-  </si>
-  <si>
     <t>hazards-title</t>
   </si>
   <si>
@@ -585,9 +570,6 @@
     <t>Additional accessibility information</t>
   </si>
   <si>
-    <t>Detailed Conformance Information:</t>
-  </si>
-  <si>
     <t>Web Accessibility Content Guidelines (WCAG) 2.1</t>
   </si>
   <si>
@@ -630,15 +612,9 @@
     <t>headings</t>
   </si>
   <si>
-    <t>The accessibility of formulas, charts, and diagrams is not available.</t>
-  </si>
-  <si>
     <t>No information about possible hazards is available.</t>
   </si>
   <si>
-    <t>The presence of hazards is unknown.</t>
-  </si>
-  <si>
     <t>No accessibility summary is available.</t>
   </si>
   <si>
@@ -678,9 +654,6 @@
     <t>Text and page layout cannot be modified as the reading experience is close to a print version, but reading systems can still provide zooming options</t>
   </si>
   <si>
-    <t>Ability to modify the appearance is not known</t>
-  </si>
-  <si>
     <t>All content is available in generated read aloud speech and electronic braille</t>
   </si>
   <si>
@@ -702,9 +675,6 @@
     <t>The conformance metadata is missing and conformity to a standard of this publication is unknown</t>
   </si>
   <si>
-    <t>For more information, refer to the certifier's report</t>
-  </si>
-  <si>
     <t>Audiobook with no text alternative</t>
   </si>
   <si>
@@ -726,9 +696,6 @@
     <t>A page list enables users to navigate directly to pages from the identified print source version</t>
   </si>
   <si>
-    <t>The accessibility of formulas, charts, and diagrams is not available</t>
-  </si>
-  <si>
     <t>Charts and diagrams are present and described by extended descriptions</t>
   </si>
   <si>
@@ -738,16 +705,19 @@
     <t>Chemistry is in an accessible format</t>
   </si>
   <si>
-    <t>formulas, charts, and diagrams without any information about the accessibility of this content</t>
-  </si>
-  <si>
-    <t>The publication contains no hazards</t>
-  </si>
-  <si>
     <t>which can cause discomfort, distraction, photosensitive seizures, or motion sickness</t>
   </si>
   <si>
     <t>The presence of hazards is unknown</t>
+  </si>
+  <si>
+    <t>For more information refer to the certifier's report</t>
+  </si>
+  <si>
+    <t>Charts, diagrams, math, and formulas</t>
+  </si>
+  <si>
+    <t>accessibility of formulas, charts, math, and diagrams not identified as being accessible</t>
   </si>
 </sst>
 </file>
@@ -1201,10 +1171,10 @@
   <dimension ref="A1:F157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B67" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C39" sqref="C39"/>
+      <selection pane="bottomRight" activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1220,19 +1190,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
@@ -1271,11 +1241,11 @@
       </c>
       <c r="C3" s="6" t="str">
         <f>IFERROR(VLOOKUP($A3,'epub-metadata-strings'!$D$2:$E$1000,2,FALSE),"")</f>
-        <v>ppearance can be modified</v>
+        <v>Appearance can be modified</v>
       </c>
       <c r="D3" s="3" t="b">
         <f t="shared" ref="D3:F66" si="0">IF($B3="","",$B3=C3)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="6" t="str">
         <f>VLOOKUP($A3,'onix-metadata-strings'!$D$2:$E$1000,2,FALSE)</f>
@@ -1317,7 +1287,7 @@
       </c>
       <c r="B5" s="6" t="str">
         <f>IFERROR(VLOOKUP($A5&amp;"-compact",'principles-string'!$A$2:$G$1000,7,FALSE),"")</f>
-        <v>Ability to modify the appearance is not known</v>
+        <v>Appearance modifiability not known</v>
       </c>
       <c r="C5" s="6" t="str">
         <f>IFERROR(VLOOKUP($A5,'epub-metadata-strings'!$D$2:$E$1000,2,FALSE),"")</f>
@@ -1325,7 +1295,7 @@
       </c>
       <c r="D5" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="6" t="str">
         <f>VLOOKUP($A5,'onix-metadata-strings'!$D$2:$E$1000,2,FALSE)</f>
@@ -1333,7 +1303,7 @@
       </c>
       <c r="F5" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -1642,7 +1612,7 @@
       </c>
       <c r="B18" s="6" t="str">
         <f>IFERROR(VLOOKUP($A18&amp;"-compact",'principles-string'!$A$2:$G$1000,7,FALSE),"")</f>
-        <v>Detailed Conformance Information:</v>
+        <v>Detailed Conformance Information</v>
       </c>
       <c r="C18" s="6" t="str">
         <f>IFERROR(VLOOKUP($A18,'epub-metadata-strings'!$D$2:$E$1000,2,FALSE),"")</f>
@@ -1650,7 +1620,7 @@
       </c>
       <c r="D18" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="6" t="str">
         <f>VLOOKUP($A18,'onix-metadata-strings'!$D$2:$E$1000,2,FALSE)</f>
@@ -1658,7 +1628,7 @@
       </c>
       <c r="F18" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1792,23 +1762,23 @@
       </c>
       <c r="B24" s="6" t="str">
         <f>IFERROR(VLOOKUP($A24&amp;"-compact",'principles-string'!$A$2:$G$1000,7,FALSE),"")</f>
-        <v>For more information, refer to the certifier's report</v>
+        <v>For more information refer to the certifier's report</v>
       </c>
       <c r="C24" s="6" t="str">
         <f>IFERROR(VLOOKUP($A24,'epub-metadata-strings'!$D$2:$E$1000,2,FALSE),"")</f>
-        <v>For more information refer to the certifier's report.</v>
+        <v>For more information refer to the certifier's report</v>
       </c>
       <c r="D24" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="6" t="str">
         <f>VLOOKUP($A24,'onix-metadata-strings'!$D$2:$E$1000,2,FALSE)</f>
-        <v>For more information refer to the certifier's report.</v>
+        <v>For more information refer to the certifier's report</v>
       </c>
       <c r="F24" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1942,7 +1912,7 @@
       </c>
       <c r="B30" s="6" t="str">
         <f>IFERROR(VLOOKUP($A30&amp;"-compact",'principles-string'!$A$2:$G$1000,7,FALSE),"")</f>
-        <v>with a credential of</v>
+        <v>The certifier's credential is</v>
       </c>
       <c r="C30" s="6" t="str">
         <f>IFERROR(VLOOKUP($A30,'epub-metadata-strings'!$D$2:$E$1000,2,FALSE),"")</f>
@@ -1950,7 +1920,7 @@
       </c>
       <c r="D30" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E30" s="6" t="str">
         <f>VLOOKUP($A30,'onix-metadata-strings'!$D$2:$E$1000,2,FALSE)</f>
@@ -1958,7 +1928,7 @@
       </c>
       <c r="F30" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -2171,19 +2141,19 @@
       </c>
       <c r="C39" s="6" t="str">
         <f>IFERROR(VLOOKUP($A39,'epub-metadata-strings'!$D$2:$E$1000,2,FALSE),"")</f>
-        <v>structural navigation</v>
+        <v>headings</v>
       </c>
       <c r="D39" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39" s="6" t="str">
         <f>VLOOKUP($A39,'onix-metadata-strings'!$D$2:$E$1000,2,FALSE)</f>
-        <v>structural navigation</v>
+        <v>headings</v>
       </c>
       <c r="F39" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -2292,11 +2262,11 @@
       </c>
       <c r="B44" s="6" t="str">
         <f>IFERROR(VLOOKUP($A44&amp;"-compact",'principles-string'!$A$2:$G$1000,7,FALSE),"")</f>
-        <v>Charts, diagrams, and formulas</v>
+        <v>Charts, diagrams, math, and formulas</v>
       </c>
       <c r="C44" s="6" t="str">
         <f>IFERROR(VLOOKUP($A44,'epub-metadata-strings'!$D$2:$E$1000,2,FALSE),"")</f>
-        <v>Charts, diagrams, and formulas</v>
+        <v>Charts, diagrams, math, and formulas</v>
       </c>
       <c r="D44" s="3" t="b">
         <f t="shared" si="0"/>
@@ -2304,7 +2274,7 @@
       </c>
       <c r="E44" s="6" t="str">
         <f>VLOOKUP($A44,'onix-metadata-strings'!$D$2:$E$1000,2,FALSE)</f>
-        <v>Charts, diagrams, and formulas</v>
+        <v>Charts, diagrams, math, and formulas</v>
       </c>
       <c r="F44" s="3" t="b">
         <f t="shared" si="0"/>
@@ -2317,23 +2287,23 @@
       </c>
       <c r="B45" s="6" t="str">
         <f>IFERROR(VLOOKUP($A45&amp;"-compact",'principles-string'!$A$2:$G$1000,7,FALSE),"")</f>
-        <v>The accessibility of formulas, charts, and diagrams is not available</v>
+        <v>accessibility of formulas, charts, math, and diagrams not identified as being accessible</v>
       </c>
       <c r="C45" s="6" t="str">
         <f>IFERROR(VLOOKUP($A45,'epub-metadata-strings'!$D$2:$E$1000,2,FALSE),"")</f>
-        <v>The accessibility of formulas, charts, and diagrams is not available.</v>
+        <v>accessibility of formulas, charts, math, and diagrams not identified as being accessible</v>
       </c>
       <c r="D45" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E45" s="6" t="str">
         <f>VLOOKUP($A45,'onix-metadata-strings'!$D$2:$E$1000,2,FALSE)</f>
-        <v>The accessibility of formulas, charts, and diagrams is not available.</v>
+        <v>accessibility of formulas, charts, math, and diagrams not identified as being accessible</v>
       </c>
       <c r="F45" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -2465,9 +2435,9 @@
       <c r="A51" t="str">
         <v>hazards-none</v>
       </c>
-      <c r="B51" s="6">
+      <c r="B51" s="6" t="str">
         <f>IFERROR(VLOOKUP($A51&amp;"-compact",'principles-string'!$A$2:$G$1000,7,FALSE),"")</f>
-        <v>0</v>
+        <v>No hazards</v>
       </c>
       <c r="C51" s="6" t="str">
         <f>IFERROR(VLOOKUP($A51,'epub-metadata-strings'!$D$2:$E$1000,2,FALSE),"")</f>
@@ -2475,7 +2445,7 @@
       </c>
       <c r="D51" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E51" s="6" t="str">
         <f>VLOOKUP($A51,'onix-metadata-strings'!$D$2:$E$1000,2,FALSE)</f>
@@ -2483,7 +2453,7 @@
       </c>
       <c r="F51" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
@@ -2546,19 +2516,19 @@
       </c>
       <c r="C54" s="6" t="str">
         <f>IFERROR(VLOOKUP($A54,'epub-metadata-strings'!$D$2:$E$1000,2,FALSE),"")</f>
-        <v>motion</v>
+        <v>motion simulation</v>
       </c>
       <c r="D54" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E54" s="6" t="str">
         <f>VLOOKUP($A54,'onix-metadata-strings'!$D$2:$E$1000,2,FALSE)</f>
-        <v>motion</v>
+        <v>motion simulation</v>
       </c>
       <c r="F54" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
@@ -2596,19 +2566,19 @@
       </c>
       <c r="C56" s="6" t="str">
         <f>IFERROR(VLOOKUP($A56,'epub-metadata-strings'!$D$2:$E$1000,2,FALSE),"")</f>
-        <v>The presence of hazards is unknown.</v>
+        <v>The presence of hazards is unknown</v>
       </c>
       <c r="D56" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E56" s="6" t="str">
         <f>VLOOKUP($A56,'onix-metadata-strings'!$D$2:$E$1000,2,FALSE)</f>
-        <v>The presence of hazards is unknown.</v>
+        <v>The presence of hazards is unknown</v>
       </c>
       <c r="F56" s="3" t="b">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
@@ -3950,8 +3920,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DAAE526-051A-2147-9F70-F78890C8D07D}">
   <dimension ref="A1:G104"/>
   <sheetViews>
-    <sheetView topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="F110" sqref="F110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3963,25 +3933,25 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E1" t="s">
         <v>135</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
+        <v>173</v>
+      </c>
+      <c r="G1" t="s">
         <v>136</v>
-      </c>
-      <c r="D1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F1" t="s">
-        <v>179</v>
-      </c>
-      <c r="G1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -3990,16 +3960,16 @@
         <v>visual-adjustments-title-compact</v>
       </c>
       <c r="C2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E2" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="G2" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -4008,16 +3978,16 @@
         <v>visual-adjustments-modifiable-descriptive</v>
       </c>
       <c r="D3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F3" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G3" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -4026,16 +3996,16 @@
         <v>visual-adjustments-unmodifiable-descriptive</v>
       </c>
       <c r="D4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F4" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G4" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -4044,16 +4014,16 @@
         <v>visual-adjustments-unknown-descriptive</v>
       </c>
       <c r="D5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F5" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G5" t="s">
-        <v>204</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -4062,16 +4032,16 @@
         <v>visual-adjustments-modifiable-compact</v>
       </c>
       <c r="D6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E6" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F6" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G6" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -4080,13 +4050,13 @@
         <v>visual-adjustments-unmodifiable-compact</v>
       </c>
       <c r="D7" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E7" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="F7" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G7" t="s">
         <v>1</v>
@@ -4098,16 +4068,16 @@
         <v>visual-adjustments-unknown-compact</v>
       </c>
       <c r="D8" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E8" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F8" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G8" t="s">
-        <v>204</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -4116,13 +4086,13 @@
         <v>nonvisual-reading-title-compact</v>
       </c>
       <c r="D9" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E9" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="G9" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -4131,16 +4101,16 @@
         <v>nonvisual-reading-readable-descriptive</v>
       </c>
       <c r="D10" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E10" t="s">
         <v>3</v>
       </c>
       <c r="F10" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G10" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -4149,16 +4119,16 @@
         <v>nonvisual-reading-may-not-fully-descriptive</v>
       </c>
       <c r="D11" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E11" t="s">
         <v>7</v>
       </c>
       <c r="F11" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G11" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -4167,16 +4137,16 @@
         <v>nonvisual-reading-not-fully-descriptive</v>
       </c>
       <c r="D12" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E12" t="s">
         <v>5</v>
       </c>
       <c r="F12" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G12" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -4185,13 +4155,13 @@
         <v>nonvisual-reading-readable-compact</v>
       </c>
       <c r="D13" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E13" t="s">
         <v>3</v>
       </c>
       <c r="F13" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G13" t="s">
         <v>4</v>
@@ -4203,13 +4173,13 @@
         <v>nonvisual-reading-may-not-fully-compact</v>
       </c>
       <c r="D14" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E14" t="s">
         <v>7</v>
       </c>
       <c r="F14" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G14" t="s">
         <v>8</v>
@@ -4221,13 +4191,13 @@
         <v>nonvisual-reading-not-fully-compact</v>
       </c>
       <c r="D15" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E15" t="s">
         <v>5</v>
       </c>
       <c r="F15" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G15" t="s">
         <v>6</v>
@@ -4239,13 +4209,13 @@
         <v>conformance-title-compact</v>
       </c>
       <c r="D16" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E16" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="G16" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -4254,13 +4224,13 @@
         <v>conformance-aaa-compact</v>
       </c>
       <c r="D17" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E17" t="s">
         <v>9</v>
       </c>
       <c r="F17" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G17" t="s">
         <v>10</v>
@@ -4272,16 +4242,16 @@
         <v>conformance-aaa-descriptive</v>
       </c>
       <c r="D18" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E18" t="s">
         <v>9</v>
       </c>
       <c r="F18" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G18" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -4290,13 +4260,13 @@
         <v>conformance-aa-compact</v>
       </c>
       <c r="D19" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E19" t="s">
         <v>11</v>
       </c>
       <c r="F19" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G19" t="s">
         <v>12</v>
@@ -4308,16 +4278,16 @@
         <v>conformance-aa-descriptive</v>
       </c>
       <c r="D20" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E20" t="s">
         <v>11</v>
       </c>
       <c r="F20" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G20" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -4326,13 +4296,13 @@
         <v>conformance-a-compact</v>
       </c>
       <c r="D21" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E21" t="s">
         <v>13</v>
       </c>
       <c r="F21" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G21" t="s">
         <v>14</v>
@@ -4344,16 +4314,16 @@
         <v>conformance-a-descriptive</v>
       </c>
       <c r="D22" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E22" t="s">
         <v>13</v>
       </c>
       <c r="F22" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G22" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -4362,13 +4332,13 @@
         <v>conformance-no-compact</v>
       </c>
       <c r="D23" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E23" t="s">
         <v>16</v>
       </c>
       <c r="F23" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G23" t="s">
         <v>17</v>
@@ -4380,16 +4350,16 @@
         <v>conformance-no-descriptive</v>
       </c>
       <c r="D24" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E24" t="s">
         <v>16</v>
       </c>
       <c r="F24" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G24" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -4398,13 +4368,13 @@
         <v>conformance-aa-compact</v>
       </c>
       <c r="D25" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E25" t="s">
         <v>11</v>
       </c>
       <c r="F25" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G25" t="s">
         <v>12</v>
@@ -4416,13 +4386,13 @@
         <v>conformance-certification-info-compact</v>
       </c>
       <c r="D26" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E26" t="s">
         <v>42</v>
       </c>
       <c r="F26" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G26" t="s">
         <v>43</v>
@@ -4434,13 +4404,13 @@
         <v>conformance-certifier-prefix-compact</v>
       </c>
       <c r="D27" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E27" t="s">
         <v>45</v>
       </c>
       <c r="F27" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G27" t="s">
         <v>46</v>
@@ -4452,13 +4422,13 @@
         <v>conformance-certifier-credentials-prefix-compact</v>
       </c>
       <c r="D28" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E28" t="s">
         <v>47</v>
       </c>
       <c r="F28" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G28" t="s">
         <v>48</v>
@@ -4470,13 +4440,13 @@
         <v>conformance-details-compact</v>
       </c>
       <c r="D29" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E29" t="s">
         <v>22</v>
       </c>
       <c r="G29" t="s">
-        <v>173</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -4485,7 +4455,7 @@
         <v>conformance-claim-compact</v>
       </c>
       <c r="D30" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E30" t="s">
         <v>24</v>
@@ -4500,7 +4470,7 @@
         <v>conformance-epub-accessibility-1-1-compact</v>
       </c>
       <c r="D31" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E31" t="s">
         <v>28</v>
@@ -4515,16 +4485,16 @@
         <v>conformance-wcag-2-1-descriptive</v>
       </c>
       <c r="D32" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E32" t="s">
         <v>32</v>
       </c>
       <c r="F32" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G32" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -4533,7 +4503,7 @@
         <v>conformance-level-aa-compact</v>
       </c>
       <c r="D33" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E33" t="s">
         <v>38</v>
@@ -4548,13 +4518,13 @@
         <v>conformance-certification-info-descriptive</v>
       </c>
       <c r="D34" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E34" t="s">
         <v>42</v>
       </c>
       <c r="F34" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G34" t="s">
         <v>43</v>
@@ -4566,10 +4536,10 @@
         <v>conformance-certification-date-prefix-compact</v>
       </c>
       <c r="D35" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E35" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G35" t="s">
         <v>44</v>
@@ -4581,13 +4551,13 @@
         <v>conformance-certifier-prefix-descriptive</v>
       </c>
       <c r="D36" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E36" t="s">
         <v>45</v>
       </c>
       <c r="F36" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G36" t="s">
         <v>46</v>
@@ -4599,7 +4569,7 @@
         <v>conformance-certifier-credentials-prefix-compact</v>
       </c>
       <c r="D37" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E37" t="s">
         <v>47</v>
@@ -4614,13 +4584,13 @@
         <v>conformance-certifier-report-compact</v>
       </c>
       <c r="D38" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E38" t="s">
         <v>49</v>
       </c>
       <c r="G38" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -4629,13 +4599,13 @@
         <v>conformance-a-compact</v>
       </c>
       <c r="D39" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E39" t="s">
         <v>13</v>
       </c>
       <c r="F39" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G39" t="s">
         <v>14</v>
@@ -4647,13 +4617,13 @@
         <v>conformance-certification-info-compact</v>
       </c>
       <c r="D40" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E40" t="s">
         <v>42</v>
       </c>
       <c r="F40" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G40" t="s">
         <v>43</v>
@@ -4665,13 +4635,13 @@
         <v>conformance-certifier-prefix-compact</v>
       </c>
       <c r="D41" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E41" t="s">
         <v>45</v>
       </c>
       <c r="F41" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G41" t="s">
         <v>46</v>
@@ -4683,13 +4653,13 @@
         <v>conformance-certifier-credentials-prefix-compact</v>
       </c>
       <c r="D42" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E42" t="s">
         <v>47</v>
       </c>
       <c r="F42" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G42" t="s">
         <v>48</v>
@@ -4701,13 +4671,13 @@
         <v>conformance-details-compact</v>
       </c>
       <c r="D43" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E43" t="s">
         <v>22</v>
       </c>
       <c r="G43" t="s">
-        <v>173</v>
+        <v>23</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -4716,7 +4686,7 @@
         <v>conformance-claim-compact</v>
       </c>
       <c r="D44" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E44" t="s">
         <v>24</v>
@@ -4731,7 +4701,7 @@
         <v>conformance-epub-accessibility-1-0-compact</v>
       </c>
       <c r="D45" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E45" t="s">
         <v>26</v>
@@ -4746,16 +4716,16 @@
         <v>conformance-wcag-2-2-descriptive</v>
       </c>
       <c r="D46" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E46" t="s">
         <v>34</v>
       </c>
       <c r="F46" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G46" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -4764,7 +4734,7 @@
         <v>conformance-level-a-compact</v>
       </c>
       <c r="D47" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E47" t="s">
         <v>40</v>
@@ -4779,13 +4749,13 @@
         <v>conformance-certification-info-descriptive</v>
       </c>
       <c r="D48" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E48" t="s">
         <v>42</v>
       </c>
       <c r="F48" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G48" t="s">
         <v>43</v>
@@ -4797,10 +4767,10 @@
         <v>conformance-certification-date-prefix-compact</v>
       </c>
       <c r="D49" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E49" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="G49" t="s">
         <v>44</v>
@@ -4812,13 +4782,13 @@
         <v>conformance-certifier-prefix-descriptive</v>
       </c>
       <c r="D50" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E50" t="s">
         <v>45</v>
       </c>
       <c r="F50" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G50" t="s">
         <v>46</v>
@@ -4830,7 +4800,7 @@
         <v>conformance-certifier-credentials-prefix-compact</v>
       </c>
       <c r="D51" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E51" t="s">
         <v>47</v>
@@ -4845,13 +4815,13 @@
         <v>conformance-certifier-report-compact</v>
       </c>
       <c r="D52" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E52" t="s">
         <v>49</v>
       </c>
       <c r="G52" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
@@ -4860,10 +4830,10 @@
         <v>conformance-unknown-standard-compact</v>
       </c>
       <c r="D53" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E53" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="G53" t="s">
         <v>15</v>
@@ -4875,7 +4845,7 @@
         <v>conformance-certifier-compact</v>
       </c>
       <c r="D54" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E54" t="s">
         <v>18</v>
@@ -4890,13 +4860,13 @@
         <v>conformance-certifier-credentials-compact</v>
       </c>
       <c r="D55" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E55" t="s">
         <v>20</v>
       </c>
       <c r="G55" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
@@ -4905,13 +4875,13 @@
         <v>conformance-no-compact</v>
       </c>
       <c r="D56" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E56" t="s">
         <v>16</v>
       </c>
       <c r="F56" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G56" t="s">
         <v>17</v>
@@ -4923,13 +4893,13 @@
         <v>pre-recorded-audio-title-compact</v>
       </c>
       <c r="D57" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E57" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="G57" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
@@ -4938,16 +4908,16 @@
         <v>pre-recorded-audio-no-metadata-descriptive</v>
       </c>
       <c r="D58" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E58" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F58" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G58" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
@@ -4956,16 +4926,16 @@
         <v>pre-recorded-audio-only-descriptive</v>
       </c>
       <c r="D59" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E59" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F59" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G59" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
@@ -4974,16 +4944,16 @@
         <v>pre-recorded-audio-complementary-descriptive</v>
       </c>
       <c r="D60" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E60" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F60" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G60" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
@@ -4992,16 +4962,16 @@
         <v>pre-recorded-audio-synchronized-descriptive</v>
       </c>
       <c r="D61" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E61" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F61" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G61" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
@@ -5010,16 +4980,16 @@
         <v>pre-recorded-audio-only-compact</v>
       </c>
       <c r="D62" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E62" t="s">
+        <v>50</v>
+      </c>
+      <c r="F62" t="s">
+        <v>176</v>
+      </c>
+      <c r="G62" t="s">
         <v>51</v>
-      </c>
-      <c r="F62" t="s">
-        <v>182</v>
-      </c>
-      <c r="G62" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
@@ -5028,16 +4998,16 @@
         <v>pre-recorded-audio-complementary-compact</v>
       </c>
       <c r="D63" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E63" t="s">
+        <v>54</v>
+      </c>
+      <c r="F63" t="s">
+        <v>176</v>
+      </c>
+      <c r="G63" t="s">
         <v>55</v>
-      </c>
-      <c r="F63" t="s">
-        <v>182</v>
-      </c>
-      <c r="G63" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
@@ -5046,16 +5016,16 @@
         <v>pre-recorded-audio-synchronized-compact</v>
       </c>
       <c r="D64" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E64" t="s">
+        <v>52</v>
+      </c>
+      <c r="F64" t="s">
+        <v>176</v>
+      </c>
+      <c r="G64" t="s">
         <v>53</v>
-      </c>
-      <c r="F64" t="s">
-        <v>182</v>
-      </c>
-      <c r="G64" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
@@ -5064,13 +5034,13 @@
         <v>navigation-title-compact</v>
       </c>
       <c r="D65" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E65" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="G65" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
@@ -5079,16 +5049,16 @@
         <v>navigation-no-metadata-descriptive</v>
       </c>
       <c r="D66" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E66" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="F66" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G66" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
@@ -5097,16 +5067,16 @@
         <v>navigation-toc-descriptive</v>
       </c>
       <c r="D67" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E67" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F67" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G67" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
@@ -5115,16 +5085,16 @@
         <v>navigation-structural-descriptive</v>
       </c>
       <c r="D68" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E68" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F68" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G68" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
@@ -5133,16 +5103,16 @@
         <v>navigation-index-descriptive</v>
       </c>
       <c r="D69" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E69" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F69" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G69" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
@@ -5151,16 +5121,16 @@
         <v>navigation-page-navigation-descriptive</v>
       </c>
       <c r="D70" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E70" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F70" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G70" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
@@ -5169,16 +5139,16 @@
         <v>navigation-intro-compact</v>
       </c>
       <c r="D71" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E71" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="F71" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G71" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
@@ -5187,16 +5157,16 @@
         <v>navigation-toc-compact</v>
       </c>
       <c r="D72" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E72" t="s">
+        <v>57</v>
+      </c>
+      <c r="F72" t="s">
+        <v>176</v>
+      </c>
+      <c r="G72" t="s">
         <v>58</v>
-      </c>
-      <c r="F72" t="s">
-        <v>182</v>
-      </c>
-      <c r="G72" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
@@ -5205,16 +5175,16 @@
         <v>navigation-structural-compact</v>
       </c>
       <c r="D73" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E73" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F73" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G73" t="s">
-        <v>187</v>
+        <v>181</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
@@ -5223,16 +5193,16 @@
         <v>navigation-index-compact</v>
       </c>
       <c r="D74" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E74" t="s">
+        <v>59</v>
+      </c>
+      <c r="F74" t="s">
+        <v>176</v>
+      </c>
+      <c r="G74" t="s">
         <v>60</v>
-      </c>
-      <c r="F74" t="s">
-        <v>182</v>
-      </c>
-      <c r="G74" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
@@ -5241,13 +5211,13 @@
         <v>join-array-and-compact</v>
       </c>
       <c r="D75" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E75" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G75" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
@@ -5256,16 +5226,16 @@
         <v>navigation-page-navigation-compact</v>
       </c>
       <c r="D76" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E76" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F76" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G76" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
@@ -5274,13 +5244,13 @@
         <v>charts-diagrams-formulas-title-compact</v>
       </c>
       <c r="D77" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E77" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="G77" t="s">
-        <v>166</v>
+        <v>216</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
@@ -5289,16 +5259,16 @@
         <v>charts-diagrams-formulas-unknown-descriptive</v>
       </c>
       <c r="D78" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E78" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F78" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G78" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
@@ -5307,16 +5277,16 @@
         <v>charts-diagrams-formulas-extended-descriptive</v>
       </c>
       <c r="D79" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E79" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F79" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G79" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
@@ -5325,16 +5295,16 @@
         <v>charts-diagrams-formulas-accessible-math-descriptive</v>
       </c>
       <c r="D80" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E80" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F80" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G80" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
@@ -5343,16 +5313,16 @@
         <v>charts-diagrams-formulas-accessible-chemistry-descriptive</v>
       </c>
       <c r="D81" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E81" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F81" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G81" t="s">
-        <v>223</v>
+        <v>212</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
@@ -5361,16 +5331,16 @@
         <v>charts-diagrams-formulas-unknown-descriptive</v>
       </c>
       <c r="D82" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E82" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F82" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G82" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
@@ -5379,16 +5349,16 @@
         <v>charts-diagrams-formulas-extended-compact</v>
       </c>
       <c r="D83" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E83" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F83" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G83" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
@@ -5397,16 +5367,16 @@
         <v>charts-diagrams-formulas-accessible-math-compact</v>
       </c>
       <c r="D84" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E84" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F84" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G84" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
@@ -5415,16 +5385,16 @@
         <v>charts-diagrams-formulas-accessible-chemistry-compact</v>
       </c>
       <c r="D85" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E85" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F85" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G85" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
@@ -5433,16 +5403,16 @@
         <v>charts-diagrams-formulas-unknown-compact</v>
       </c>
       <c r="D86" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E86" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="F86" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G86" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.2">
@@ -5451,13 +5421,13 @@
         <v>hazards-title-compact</v>
       </c>
       <c r="D87" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E87" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="G87" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.2">
@@ -5466,16 +5436,16 @@
         <v>hazards-no-metadata-descriptive</v>
       </c>
       <c r="D88" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E88" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F88" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G88" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.2">
@@ -5484,16 +5454,16 @@
         <v>hazards-none-descriptive</v>
       </c>
       <c r="D89" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E89" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F89" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G89" t="s">
-        <v>225</v>
+        <v>75</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.2">
@@ -5502,16 +5472,16 @@
         <v>hazards-flashing-descriptive</v>
       </c>
       <c r="D90" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E90" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F90" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G90" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.2">
@@ -5520,16 +5490,16 @@
         <v>hazards-sound-descriptive</v>
       </c>
       <c r="D91" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E91" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="F91" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G91" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.2">
@@ -5538,16 +5508,16 @@
         <v>hazards-motion-descriptive</v>
       </c>
       <c r="D92" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E92" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F92" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G92" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.2">
@@ -5556,16 +5526,16 @@
         <v>hasards-explanatory-descriptive</v>
       </c>
       <c r="D93" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E93" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="F93" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G93" t="s">
-        <v>226</v>
+        <v>213</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.2">
@@ -5574,16 +5544,16 @@
         <v>hazards-unknown-descriptive</v>
       </c>
       <c r="D94" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E94" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F94" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G94" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.2">
@@ -5592,13 +5562,16 @@
         <v>hazards-none-compact</v>
       </c>
       <c r="D95" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E95" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F95" t="s">
-        <v>182</v>
+        <v>176</v>
+      </c>
+      <c r="G95" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.2">
@@ -5607,16 +5580,16 @@
         <v>hazards-flashing-compact</v>
       </c>
       <c r="D96" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E96" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F96" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G96" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.2">
@@ -5625,13 +5598,13 @@
         <v>join-array-and-compact</v>
       </c>
       <c r="D97" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E97" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G97" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.2">
@@ -5640,16 +5613,16 @@
         <v>hazards-motion-compact</v>
       </c>
       <c r="D98" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E98" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F98" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G98" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.2">
@@ -5658,13 +5631,13 @@
         <v>hazards-plural-compact</v>
       </c>
       <c r="D99" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E99" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="G99" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.2">
@@ -5673,16 +5646,16 @@
         <v>hazards-unknown-compact</v>
       </c>
       <c r="D100" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E100" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="F100" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="G100" t="s">
-        <v>227</v>
+        <v>214</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.2">
@@ -5691,13 +5664,13 @@
         <v>accessibility-summary-title-compact</v>
       </c>
       <c r="D101" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E101" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="G101" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.2">
@@ -5706,16 +5679,16 @@
         <v>accessibility-summary-no-metadata-descriptive</v>
       </c>
       <c r="D102" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E102" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F102" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="G102" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.2">
@@ -5724,13 +5697,13 @@
         <v>legal-considerations-title-compact</v>
       </c>
       <c r="D103" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E103" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="G103" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.2">
@@ -5739,13 +5712,13 @@
         <v>additional-accessibility-information-title-compact</v>
       </c>
       <c r="D104" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E104" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="G104" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
   </sheetData>
@@ -5757,8 +5730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3555E2ED-EB14-6D43-B054-42CEC3458CC1}">
   <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E88" sqref="E88"/>
+    <sheetView topLeftCell="A66" workbookViewId="0">
+      <selection sqref="A1:E80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5769,63 +5742,63 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" t="s">
         <v>135</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>136</v>
-      </c>
-      <c r="C1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D3" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="E3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E4" t="s">
-        <v>142</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E5" t="s">
         <v>1</v>
@@ -5833,10 +5806,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E6" t="s">
         <v>2</v>
@@ -5844,18 +5817,18 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D7" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E7" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D8" t="s">
         <v>3</v>
@@ -5866,7 +5839,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D9" t="s">
         <v>5</v>
@@ -5877,7 +5850,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
@@ -5888,18 +5861,18 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D11" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E11" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D12" t="s">
         <v>9</v>
@@ -5910,7 +5883,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D13" t="s">
         <v>11</v>
@@ -5921,7 +5894,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D14" t="s">
         <v>13</v>
@@ -5932,10 +5905,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D15" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="E15" t="s">
         <v>15</v>
@@ -5943,7 +5916,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D16" t="s">
         <v>16</v>
@@ -5954,7 +5927,7 @@
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D17" t="s">
         <v>18</v>
@@ -5965,7 +5938,7 @@
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
@@ -5976,7 +5949,7 @@
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D19" t="s">
         <v>22</v>
@@ -5987,7 +5960,7 @@
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D20" t="s">
         <v>24</v>
@@ -5998,7 +5971,7 @@
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D21" t="s">
         <v>26</v>
@@ -6009,7 +5982,7 @@
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D22" t="s">
         <v>28</v>
@@ -6020,7 +5993,7 @@
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D23" t="s">
         <v>34</v>
@@ -6031,7 +6004,7 @@
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D24" t="s">
         <v>32</v>
@@ -6042,7 +6015,7 @@
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D25" t="s">
         <v>30</v>
@@ -6053,7 +6026,7 @@
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D26" t="s">
         <v>36</v>
@@ -6064,7 +6037,7 @@
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D27" t="s">
         <v>38</v>
@@ -6075,7 +6048,7 @@
     </row>
     <row r="28" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C28" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D28" t="s">
         <v>40</v>
@@ -6086,7 +6059,7 @@
     </row>
     <row r="29" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D29" t="s">
         <v>42</v>
@@ -6097,10 +6070,10 @@
     </row>
     <row r="30" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D30" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E30" t="s">
         <v>44</v>
@@ -6108,7 +6081,7 @@
     </row>
     <row r="31" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D31" t="s">
         <v>45</v>
@@ -6119,7 +6092,7 @@
     </row>
     <row r="32" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C32" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D32" t="s">
         <v>47</v>
@@ -6130,530 +6103,530 @@
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C33" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D33" t="s">
         <v>49</v>
       </c>
       <c r="E33" t="s">
-        <v>50</v>
+        <v>215</v>
       </c>
     </row>
     <row r="34" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C34" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D34" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E34" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C35" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D35" t="s">
+        <v>50</v>
+      </c>
+      <c r="E35" t="s">
         <v>51</v>
-      </c>
-      <c r="E35" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="36" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C36" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D36" t="s">
+        <v>52</v>
+      </c>
+      <c r="E36" t="s">
         <v>53</v>
-      </c>
-      <c r="E36" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C37" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D37" t="s">
+        <v>54</v>
+      </c>
+      <c r="E37" t="s">
         <v>55</v>
-      </c>
-      <c r="E37" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C38" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D38" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E38" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C39" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D39" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E39" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="40" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C40" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D40" t="s">
+        <v>57</v>
+      </c>
+      <c r="E40" t="s">
         <v>58</v>
-      </c>
-      <c r="E40" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C41" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D41" t="s">
+        <v>59</v>
+      </c>
+      <c r="E41" t="s">
         <v>60</v>
-      </c>
-      <c r="E41" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="42" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C42" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D42" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E42" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="43" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C43" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D43" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E43" t="s">
-        <v>65</v>
+        <v>181</v>
       </c>
     </row>
     <row r="44" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C44" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D44" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E44" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="45" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C45" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D45" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E45" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="46" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C46" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D46" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E46" t="s">
-        <v>166</v>
+        <v>216</v>
       </c>
     </row>
     <row r="47" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C47" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D47" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E47" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="48" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C48" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D48" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E48" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="49" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C49" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D49" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E49" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="50" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C50" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D50" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E50" t="s">
-        <v>188</v>
+        <v>217</v>
       </c>
     </row>
     <row r="51" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C51" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D51" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E51" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="52" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C52" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D52" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E52" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="53" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C53" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D53" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E53" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="54" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C54" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D54" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E54" t="s">
-        <v>81</v>
+        <v>187</v>
       </c>
     </row>
     <row r="55" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C55" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D55" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E55" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="56" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C56" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D56" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E56" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="57" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C57" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D57" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E57" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="58" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C58" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D58" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E58" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
     </row>
     <row r="59" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C59" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D59" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E59" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
     </row>
     <row r="60" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C60" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D60" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="E60" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="61" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C61" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D61" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E61" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
     </row>
     <row r="62" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C62" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D62" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="E62" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
     </row>
     <row r="63" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C63" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D63" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E63" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="64" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C64" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D64" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E64" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="65" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C65" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D65" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E65" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="66" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C66" t="s">
+        <v>138</v>
+      </c>
+      <c r="D66" t="s">
+        <v>140</v>
+      </c>
+      <c r="E66" t="s">
         <v>141</v>
-      </c>
-      <c r="D66" t="s">
-        <v>144</v>
-      </c>
-      <c r="E66" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="67" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C67" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D67" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E67" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="68" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C68" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D68" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E68" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="69" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C69" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D69" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="E69" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
     </row>
     <row r="70" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C70" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D70" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="E70" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="71" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C71" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D71" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E71" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="72" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C72" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D72" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E72" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="73" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C73" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D73" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E73" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
     </row>
     <row r="74" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C74" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D74" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="E74" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="75" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C75" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D75" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E75" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="76" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C76" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D76" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E76" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="77" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C77" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D77" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E77" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="78" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C78" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D78" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E78" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="79" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C79" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D79" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="E79" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="80" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C80" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D80" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E80" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>
@@ -6665,8 +6638,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5824B443-C64F-5248-8FD1-CED7D8535BBE}">
   <dimension ref="A1:E76"/>
   <sheetViews>
-    <sheetView topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="D93" sqref="D93"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection sqref="A1:E76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6677,63 +6650,63 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1" t="s">
         <v>135</v>
       </c>
-      <c r="B1" t="s">
+      <c r="E1" t="s">
         <v>136</v>
-      </c>
-      <c r="C1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D1" t="s">
-        <v>138</v>
-      </c>
-      <c r="E1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D3" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="E3" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C5" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E5" t="s">
         <v>1</v>
@@ -6741,10 +6714,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D6" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E6" t="s">
         <v>2</v>
@@ -6752,18 +6725,18 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D7" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E7" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D8" t="s">
         <v>3</v>
@@ -6774,7 +6747,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D9" t="s">
         <v>5</v>
@@ -6785,7 +6758,7 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
@@ -6796,18 +6769,18 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D11" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E11" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D12" t="s">
         <v>9</v>
@@ -6818,7 +6791,7 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D13" t="s">
         <v>11</v>
@@ -6829,7 +6802,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D14" t="s">
         <v>13</v>
@@ -6840,7 +6813,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C15" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D15" t="s">
         <v>16</v>
@@ -6851,7 +6824,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D16" t="s">
         <v>18</v>
@@ -6862,7 +6835,7 @@
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D17" t="s">
         <v>20</v>
@@ -6873,7 +6846,7 @@
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D18" t="s">
         <v>22</v>
@@ -6884,7 +6857,7 @@
     </row>
     <row r="19" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D19" t="s">
         <v>24</v>
@@ -6895,7 +6868,7 @@
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D20" t="s">
         <v>26</v>
@@ -6906,7 +6879,7 @@
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C21" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D21" t="s">
         <v>28</v>
@@ -6917,7 +6890,7 @@
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C22" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D22" t="s">
         <v>34</v>
@@ -6928,7 +6901,7 @@
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C23" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D23" t="s">
         <v>32</v>
@@ -6939,7 +6912,7 @@
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C24" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D24" t="s">
         <v>30</v>
@@ -6950,7 +6923,7 @@
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C25" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D25" t="s">
         <v>36</v>
@@ -6961,7 +6934,7 @@
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D26" t="s">
         <v>38</v>
@@ -6972,7 +6945,7 @@
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C27" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D27" t="s">
         <v>40</v>
@@ -6983,7 +6956,7 @@
     </row>
     <row r="28" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C28" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D28" t="s">
         <v>42</v>
@@ -6994,10 +6967,10 @@
     </row>
     <row r="29" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C29" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D29" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="E29" t="s">
         <v>44</v>
@@ -7005,7 +6978,7 @@
     </row>
     <row r="30" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C30" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D30" t="s">
         <v>45</v>
@@ -7016,7 +6989,7 @@
     </row>
     <row r="31" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C31" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D31" t="s">
         <v>47</v>
@@ -7027,497 +7000,497 @@
     </row>
     <row r="32" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C32" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D32" t="s">
         <v>49</v>
       </c>
       <c r="E32" t="s">
-        <v>50</v>
+        <v>215</v>
       </c>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C33" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D33" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E33" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="34" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C34" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D34" t="s">
+        <v>50</v>
+      </c>
+      <c r="E34" t="s">
         <v>51</v>
-      </c>
-      <c r="E34" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C35" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D35" t="s">
+        <v>54</v>
+      </c>
+      <c r="E35" t="s">
         <v>55</v>
-      </c>
-      <c r="E35" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="36" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C36" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D36" t="s">
+        <v>52</v>
+      </c>
+      <c r="E36" t="s">
         <v>53</v>
-      </c>
-      <c r="E36" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C37" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D37" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E37" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C38" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D38" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E38" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C39" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D39" t="s">
+        <v>57</v>
+      </c>
+      <c r="E39" t="s">
         <v>58</v>
-      </c>
-      <c r="E39" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="40" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C40" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D40" t="s">
+        <v>59</v>
+      </c>
+      <c r="E40" t="s">
         <v>60</v>
-      </c>
-      <c r="E40" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C41" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D41" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E41" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="42" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C42" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D42" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E42" t="s">
-        <v>65</v>
+        <v>181</v>
       </c>
     </row>
     <row r="43" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C43" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D43" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E43" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="44" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C44" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D44" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E44" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
     </row>
     <row r="45" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C45" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D45" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E45" t="s">
-        <v>166</v>
+        <v>216</v>
       </c>
     </row>
     <row r="46" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C46" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D46" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E46" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="47" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C47" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D47" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="E47" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="48" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C48" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D48" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E48" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="49" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C49" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D49" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E49" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="50" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C50" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D50" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="E50" t="s">
-        <v>188</v>
+        <v>217</v>
       </c>
     </row>
     <row r="51" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C51" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D51" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E51" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="52" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C52" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D52" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E52" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="53" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C53" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D53" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E53" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="54" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C54" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D54" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E54" t="s">
-        <v>81</v>
+        <v>187</v>
       </c>
     </row>
     <row r="55" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C55" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D55" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E55" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="56" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C56" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D56" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="E56" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="57" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C57" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D57" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E57" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="58" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C58" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D58" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E58" t="s">
-        <v>190</v>
+        <v>214</v>
       </c>
     </row>
     <row r="59" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C59" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D59" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E59" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
     </row>
     <row r="60" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C60" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D60" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="E60" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
     </row>
     <row r="61" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C61" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D61" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E61" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
     </row>
     <row r="62" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C62" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D62" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="E62" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
     </row>
     <row r="63" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C63" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D63" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E63" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="64" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C64" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D64" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E64" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="65" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C65" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D65" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="E65" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="66" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C66" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D66" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E66" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="67" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C67" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D67" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E67" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="68" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C68" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D68" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E68" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="69" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C69" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D69" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E69" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="70" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C70" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D70" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E70" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="71" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C71" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D71" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E71" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="72" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C72" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D72" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E72" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="73" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C73" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D73" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="E73" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="74" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C74" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D74" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="E74" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="75" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C75" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D75" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E75" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="76" spans="3:5" x14ac:dyDescent="0.2">
       <c r="C76" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D76" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E76" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>